<commit_message>
Fixed blowup but KO panel screwed for formate
</commit_message>
<xml_diff>
--- a/Paper/excel figures.xlsx
+++ b/Paper/excel figures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="108" windowWidth="16260" windowHeight="8736" activeTab="3"/>
+    <workbookView xWindow="390" yWindow="105" windowWidth="16260" windowHeight="8730"/>
   </bookViews>
   <sheets>
     <sheet name="Growth Yield" sheetId="4" r:id="rId1"/>
@@ -307,13 +307,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,11 +483,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="75614848"/>
-        <c:axId val="75616640"/>
+        <c:axId val="49810048"/>
+        <c:axId val="49811840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75614848"/>
+        <c:axId val="49810048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -496,7 +496,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75616640"/>
+        <c:crossAx val="49811840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -504,7 +504,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75616640"/>
+        <c:axId val="49811840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -515,7 +515,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75614848"/>
+        <c:crossAx val="49810048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -859,15 +859,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E22"/>
+  <dimension ref="A2:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -937,9 +937,15 @@
         <v>2.02</v>
       </c>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <f>-1226.2-2077.7+2011.4+1296.8</f>
+        <v>4.3000000000004093</v>
       </c>
     </row>
   </sheetData>
@@ -953,17 +959,17 @@
   <dimension ref="B1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B1" sqref="B1:G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.21875" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -980,7 +986,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -997,7 +1003,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1014,7 +1020,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1031,7 +1037,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1048,7 +1054,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1065,7 +1071,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
@@ -1082,7 +1088,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1099,7 +1105,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1116,7 +1122,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -1133,7 +1139,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1150,7 +1156,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1167,7 +1173,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1184,7 +1190,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1201,7 +1207,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1218,7 +1224,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1234,31 +1240,31 @@
       <c r="F16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
+    <row r="17" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B17" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>39</v>
       </c>
@@ -1274,22 +1280,22 @@
   <dimension ref="A2:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B2" sqref="B2:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.21875" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1406,6 +1412,7 @@
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1413,11 +1420,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Expanded KO panel code to all and altered KO figure
</commit_message>
<xml_diff>
--- a/Paper/excel figures.xlsx
+++ b/Paper/excel figures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="105" windowWidth="16260" windowHeight="8730"/>
+    <workbookView xWindow="390" yWindow="105" windowWidth="16260" windowHeight="8730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Growth Yield" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="54">
   <si>
     <t>KO Genes</t>
   </si>
@@ -82,16 +82,10 @@
     <t>10 of 10</t>
   </si>
   <si>
-    <t>13 of 13</t>
-  </si>
-  <si>
     <t>2 of 2</t>
   </si>
   <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>27 of 27</t>
   </si>
   <si>
     <t>Internal Reactions</t>
@@ -190,12 +184,54 @@
   <si>
     <t>Figure 1. Comparison of predicted and experimental growth yields</t>
   </si>
+  <si>
+    <t>1 of 2</t>
+  </si>
+  <si>
+    <t>∆hdrB2</t>
+  </si>
+  <si>
+    <r>
+      <t>∆6H2ase</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>supp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>∆7H2ase</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>supp</t>
+    </r>
+  </si>
+  <si>
+    <t>14 of 16</t>
+  </si>
+  <si>
+    <t>27 of 30</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,8 +269,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,6 +294,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -286,10 +342,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -314,9 +371,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -483,11 +543,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="49810048"/>
-        <c:axId val="49811840"/>
+        <c:axId val="97425280"/>
+        <c:axId val="97426816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="49810048"/>
+        <c:axId val="97425280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -496,7 +556,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49811840"/>
+        <c:crossAx val="97426816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -504,7 +564,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49811840"/>
+        <c:axId val="97426816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -515,7 +575,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49810048"/>
+        <c:crossAx val="97425280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -861,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,7 +932,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -880,7 +940,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>4.2300000000000004</v>
@@ -891,7 +951,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>2.86</v>
@@ -902,7 +962,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B5">
         <v>0.57999999999999996</v>
@@ -913,7 +973,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6">
         <f>B4+B5</f>
@@ -926,7 +986,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <f>B4-B5</f>
@@ -939,7 +999,7 @@
     </row>
     <row r="22" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="5:6" x14ac:dyDescent="0.25">
@@ -956,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G19"/>
+  <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,7 +1029,7 @@
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -986,287 +1046,344 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B20" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B17" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="10" t="s">
+      <c r="C20" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D20" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>39</v>
+      <c r="F20" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="15">
+        <f>27/30</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1292,7 +1409,7 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -1301,20 +1418,20 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="5">
         <v>494</v>
@@ -1327,7 +1444,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C5" s="5">
         <v>29</v>
@@ -1340,20 +1457,20 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C7" s="5">
         <v>266</v>
@@ -1366,7 +1483,7 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C8" s="5">
         <v>610</v>
@@ -1379,7 +1496,7 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="5">
         <v>52</v>
@@ -1392,7 +1509,7 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="4">
         <v>485</v>
@@ -1404,7 +1521,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added transportDB genes but not finished
</commit_message>
<xml_diff>
--- a/Paper/excel figures.xlsx
+++ b/Paper/excel figures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="396" yWindow="108" windowWidth="15576" windowHeight="8736"/>
+    <workbookView xWindow="390" yWindow="105" windowWidth="15570" windowHeight="8730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Growth Yield" sheetId="4" r:id="rId1"/>
@@ -543,11 +543,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="56115584"/>
-        <c:axId val="56117120"/>
+        <c:axId val="91265280"/>
+        <c:axId val="91279360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="56115584"/>
+        <c:axId val="91265280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -556,7 +556,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56117120"/>
+        <c:crossAx val="91279360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -564,7 +564,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56117120"/>
+        <c:axId val="91279360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -575,7 +575,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56115584"/>
+        <c:crossAx val="91265280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -921,16 +921,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>46</v>
       </c>
@@ -938,7 +938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -949,7 +949,7 @@
         <v>3.89</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -960,7 +960,7 @@
         <v>2.31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -971,7 +971,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -984,7 +984,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -997,12 +997,12 @@
         <v>2.02</v>
       </c>
     </row>
-    <row r="22" spans="5:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="F30">
         <f>-1226.2-2077.7+2011.4+1296.8</f>
         <v>4.3000000000004093</v>
@@ -1018,18 +1018,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>49</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>50</v>
       </c>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="G18" s="12"/>
     </row>
-    <row r="19" spans="2:8" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>51</v>
       </c>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="G19" s="12"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
         <v>40</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>37</v>
       </c>
@@ -1400,10 +1400,10 @@
       <selection activeCell="B2" sqref="B2:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1541,7 +1541,7 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Various updates needing MeOH investigation
</commit_message>
<xml_diff>
--- a/Paper/excel figures.xlsx
+++ b/Paper/excel figures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="105" windowWidth="15570" windowHeight="8730" activeTab="1"/>
+    <workbookView xWindow="396" yWindow="108" windowWidth="15576" windowHeight="8736"/>
   </bookViews>
   <sheets>
     <sheet name="Growth Yield" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="57">
   <si>
     <t>KO Genes</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Gene-Associated Reactions</t>
   </si>
   <si>
-    <t>iMR494</t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
@@ -115,13 +112,7 @@
     <t>556/49</t>
   </si>
   <si>
-    <t>635/52</t>
-  </si>
-  <si>
     <t>% ORF Coverage</t>
-  </si>
-  <si>
-    <t>Table 1. A comparison between iMR494 and iMM518</t>
   </si>
   <si>
     <r>
@@ -225,6 +216,24 @@
   </si>
   <si>
     <t>27 of 30</t>
+  </si>
+  <si>
+    <t>MCC</t>
+  </si>
+  <si>
+    <t>iMR524</t>
+  </si>
+  <si>
+    <t>646/45</t>
+  </si>
+  <si>
+    <t>Table 1. A comparison between iMR524 and iMM518</t>
+  </si>
+  <si>
+    <t>Model Error</t>
+  </si>
+  <si>
+    <t>Model Top Error</t>
   </si>
 </sst>
 </file>
@@ -543,11 +552,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="91265280"/>
-        <c:axId val="91279360"/>
+        <c:axId val="135644672"/>
+        <c:axId val="135646208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91265280"/>
+        <c:axId val="135644672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -556,7 +565,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91279360"/>
+        <c:crossAx val="135646208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -564,7 +573,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91279360"/>
+        <c:axId val="135646208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -575,7 +584,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91265280"/>
+        <c:crossAx val="135644672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -921,26 +930,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>3.89</v>
@@ -949,9 +958,9 @@
         <v>3.89</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <v>2.86</v>
@@ -960,9 +969,9 @@
         <v>2.31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>0.57999999999999996</v>
@@ -971,9 +980,9 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <f>B4+B5</f>
@@ -984,9 +993,9 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B7">
         <f>B4-B5</f>
@@ -997,12 +1006,38 @@
         <v>2.02</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="14">
+        <f>(B3-B4)/B4</f>
+        <v>0.36013986013986027</v>
+      </c>
+      <c r="C8" s="14">
+        <f>(C3-C4)/C4</f>
+        <v>0.68398268398268403</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="14">
+        <f>(B3-B6)/B6</f>
+        <v>0.13081395348837216</v>
+      </c>
+      <c r="C9" s="14">
+        <f>(C3-C6)/C6</f>
+        <v>0.49615384615384617</v>
+      </c>
+    </row>
     <row r="22" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="5:6" ht="14.45" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="5:6" x14ac:dyDescent="0.3">
       <c r="F30">
         <f>-1226.2-2077.7+2011.4+1296.8</f>
         <v>4.3000000000004093</v>
@@ -1018,18 +1053,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1046,344 +1081,349 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="B18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="2:8" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="B19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G19" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" s="12"/>
-    </row>
-    <row r="20" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>21</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H20" s="14">
         <f>27/30</f>
         <v>0.9</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1396,20 +1436,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -1418,23 +1458,23 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="5">
-        <v>494</v>
+        <v>524</v>
       </c>
       <c r="D4" s="5">
         <v>518</v>
@@ -1444,10 +1484,10 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="5">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5" s="5">
         <v>30</v>
@@ -1457,23 +1497,23 @@
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C7" s="5">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D7" s="5">
         <v>163</v>
@@ -1486,7 +1526,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="5">
-        <v>610</v>
+        <v>545</v>
       </c>
       <c r="D8" s="5">
         <v>570</v>
@@ -1499,7 +1539,7 @@
         <v>24</v>
       </c>
       <c r="C9" s="5">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D9" s="5">
         <v>49</v>
@@ -1512,7 +1552,7 @@
         <v>25</v>
       </c>
       <c r="C10" s="4">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="D10" s="4">
         <v>464</v>
@@ -1521,7 +1561,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1541,7 +1581,7 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated figures and almost done with PABA syn
</commit_message>
<xml_diff>
--- a/Paper/excel figures.xlsx
+++ b/Paper/excel figures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="396" yWindow="108" windowWidth="15576" windowHeight="8736"/>
+    <workbookView xWindow="390" yWindow="105" windowWidth="15570" windowHeight="8730" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Growth Yield" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="63">
   <si>
     <t>KO Genes</t>
   </si>
@@ -221,19 +221,59 @@
     <t>MCC</t>
   </si>
   <si>
-    <t>iMR524</t>
-  </si>
-  <si>
-    <t>646/45</t>
-  </si>
-  <si>
-    <t>Table 1. A comparison between iMR524 and iMM518</t>
-  </si>
-  <si>
     <t>Model Error</t>
   </si>
   <si>
     <t>Model Top Error</t>
+  </si>
+  <si>
+    <t>iMR533</t>
+  </si>
+  <si>
+    <t>656/52</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Methanococcus maripaludis S2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> model statistics</t>
+    </r>
+  </si>
+  <si>
+    <t>Transport/Exchange Reactions</t>
+  </si>
+  <si>
+    <t>58/57</t>
+  </si>
+  <si>
+    <t>Dead End Reactions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 1A. A comparison between iMR533 and iMM518 indicates that our model covers slightly more of the genome, including over 100 more gene-associated reactions. Both models include approximately the same number of reactions, but our model has roughly 100 more internal metabolites and dead end metabolites. Though this represent the portion of metabolism that cannot carry flux, all of our model's dead end metabolites are part of gene-associated reactions and thus represent promising avenues for future model expansion. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 1B. Some basic statistics for the iMR533 model. Our model has the largest genome coverage of any existing methanogen model and </t>
+  </si>
+  <si>
+    <t>% Reactions Associated with Genes (non-exchange)</t>
   </si>
 </sst>
 </file>
@@ -355,7 +395,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -370,9 +410,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -381,6 +418,13 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -552,11 +596,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="135644672"/>
-        <c:axId val="135646208"/>
+        <c:axId val="82556800"/>
+        <c:axId val="82558336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="135644672"/>
+        <c:axId val="82556800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -565,7 +609,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135646208"/>
+        <c:crossAx val="82558336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -573,7 +617,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135646208"/>
+        <c:axId val="82558336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -584,7 +628,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135644672"/>
+        <c:crossAx val="82556800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -930,16 +974,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>43</v>
       </c>
@@ -947,7 +991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -958,7 +1002,7 @@
         <v>3.89</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -969,7 +1013,7 @@
         <v>2.31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -980,7 +1024,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -993,7 +1037,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1006,38 +1050,38 @@
         <v>2.02</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="14">
+        <v>52</v>
+      </c>
+      <c r="B8" s="13">
         <f>(B3-B4)/B4</f>
         <v>0.36013986013986027</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="13">
         <f>(C3-C4)/C4</f>
         <v>0.68398268398268403</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="14">
+        <v>53</v>
+      </c>
+      <c r="B9" s="13">
         <f>(B3-B6)/B6</f>
         <v>0.13081395348837216</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="13">
         <f>(C3-C6)/C6</f>
         <v>0.49615384615384617</v>
       </c>
     </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="F30">
         <f>-1226.2-2077.7+2011.4+1296.8</f>
         <v>4.3000000000004093</v>
@@ -1054,17 +1098,17 @@
   <dimension ref="B1:H22"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1081,7 +1125,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1098,7 +1142,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1115,7 +1159,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1132,7 +1176,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1149,7 +1193,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1166,7 +1210,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
@@ -1183,7 +1227,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>46</v>
       </c>
@@ -1200,7 +1244,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1217,7 +1261,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1234,7 +1278,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1251,7 +1295,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1268,7 +1312,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1285,7 +1329,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1302,14 +1346,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>35</v>
       </c>
       <c r="E15" s="3" t="s">
@@ -1319,14 +1363,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="12" t="s">
         <v>35</v>
       </c>
       <c r="E16" s="3" t="s">
@@ -1335,8 +1379,11 @@
       <c r="F16" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H16" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1349,17 +1396,14 @@
       <c r="E17" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" t="s">
-        <v>51</v>
+      <c r="F17" s="12" t="s">
+        <v>35</v>
       </c>
       <c r="H17">
         <v>0.67</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>47</v>
       </c>
@@ -1375,9 +1419,9 @@
       <c r="F18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="12"/>
-    </row>
-    <row r="19" spans="2:8" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>48</v>
       </c>
@@ -1393,35 +1437,35 @@
       <c r="F19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="9" t="s">
+    <row r="20" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B20" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="13">
         <f>27/30</f>
         <v>0.9</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>34</v>
       </c>
@@ -1434,139 +1478,293 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E12"/>
+  <dimension ref="A2:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="5">
-        <v>524</v>
+        <v>533</v>
       </c>
       <c r="D4" s="5">
         <v>518</v>
       </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="5">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" s="5">
         <v>30</v>
       </c>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C7" s="5">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D7" s="5">
         <v>163</v>
       </c>
       <c r="E7" s="6"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="5">
-        <v>545</v>
+        <v>574</v>
       </c>
       <c r="D8" s="5">
         <v>570</v>
       </c>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="5">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D9" s="5">
         <v>49</v>
       </c>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="4">
-        <v>489</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="C10" s="5">
+        <v>565</v>
+      </c>
+      <c r="D10" s="5">
         <v>464</v>
       </c>
       <c r="E10" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="8" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="4">
+        <v>89</v>
+      </c>
+      <c r="D11" s="4">
+        <v>75</v>
+      </c>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>54</v>
       </c>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="5">
+        <v>533</v>
+      </c>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="5">
+        <v>31</v>
+      </c>
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="5">
+        <v>265</v>
+      </c>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="5">
+        <v>574</v>
+      </c>
+      <c r="D25" s="5"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="5">
+        <v>218</v>
+      </c>
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="4">
+        <v>565</v>
+      </c>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="17"/>
+    </row>
+    <row r="30" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
+    <mergeCell ref="B29:C33"/>
     <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B12:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1581,7 +1779,7 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added thermo to growth sims, changed some bounds, started paper
</commit_message>
<xml_diff>
--- a/Paper/excel figures.xlsx
+++ b/Paper/excel figures.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="64">
   <si>
     <t>KO Genes</t>
   </si>
@@ -230,9 +230,6 @@
     <t>iMR533</t>
   </si>
   <si>
-    <t>656/52</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -267,13 +264,19 @@
     <t>Dead End Reactions</t>
   </si>
   <si>
-    <t xml:space="preserve">Table 1A. A comparison between iMR533 and iMM518 indicates that our model covers slightly more of the genome, including over 100 more gene-associated reactions. Both models include approximately the same number of reactions, but our model has roughly 100 more internal metabolites and dead end metabolites. Though this represent the portion of metabolism that cannot carry flux, all of our model's dead end metabolites are part of gene-associated reactions and thus represent promising avenues for future model expansion. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Table 1B. Some basic statistics for the iMR533 model. Our model has the largest genome coverage of any existing methanogen model and </t>
-  </si>
-  <si>
     <t>% Reactions Associated with Genes (non-exchange)</t>
+  </si>
+  <si>
+    <t>iMR534</t>
+  </si>
+  <si>
+    <t>650/52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 1A. A comparison between iMR533 and iMM518 indicates that our model covers slightly more of the genome, including over 100 more gene-associated reactions. Both models include approximately the same number of reactions, but our model has approximately 100 more internal metabolites and dead end metabolites. Though this represent the portion of metabolism that cannot carry flux, all of our model's dead end metabolites are part of gene-associated reactions and thus represent promising avenues for future model expansion. </t>
+  </si>
+  <si>
+    <t>Table 1B. Some basic statistics for the iMR533 model.</t>
   </si>
 </sst>
 </file>
@@ -416,15 +419,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -596,11 +599,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="82556800"/>
-        <c:axId val="82558336"/>
+        <c:axId val="104118144"/>
+        <c:axId val="104119680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82556800"/>
+        <c:axId val="104118144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -609,7 +612,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82558336"/>
+        <c:crossAx val="104119680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -617,7 +620,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82558336"/>
+        <c:axId val="104119680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -628,14 +631,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82556800"/>
+        <c:crossAx val="104118144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1481,7 +1483,7 @@
   <dimension ref="A2:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B2" sqref="B2:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,11 +1494,11 @@
   <sheetData>
     <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -1505,12 +1507,11 @@
         <v>26</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="6"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
@@ -1518,12 +1519,11 @@
         <v>27</v>
       </c>
       <c r="C4" s="5">
-        <v>533</v>
+        <v>518</v>
       </c>
       <c r="D4" s="5">
-        <v>518</v>
-      </c>
-      <c r="E4" s="6"/>
+        <v>534</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
@@ -1531,12 +1531,11 @@
         <v>31</v>
       </c>
       <c r="C5" s="5">
+        <v>30</v>
+      </c>
+      <c r="D5" s="5">
         <v>31</v>
       </c>
-      <c r="D5" s="5">
-        <v>30</v>
-      </c>
-      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
@@ -1544,12 +1543,11 @@
         <v>29</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="6"/>
+        <v>61</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
@@ -1557,12 +1555,11 @@
         <v>33</v>
       </c>
       <c r="C7" s="5">
-        <v>265</v>
+        <v>163</v>
       </c>
       <c r="D7" s="5">
-        <v>163</v>
-      </c>
-      <c r="E7" s="6"/>
+        <v>268</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
@@ -1570,12 +1567,11 @@
         <v>23</v>
       </c>
       <c r="C8" s="5">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="D8" s="5">
-        <v>570</v>
-      </c>
-      <c r="E8" s="6"/>
+        <v>571</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
@@ -1583,12 +1579,11 @@
         <v>24</v>
       </c>
       <c r="C9" s="5">
+        <v>49</v>
+      </c>
+      <c r="D9" s="5">
         <v>57</v>
       </c>
-      <c r="D9" s="5">
-        <v>49</v>
-      </c>
-      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
@@ -1596,32 +1591,30 @@
         <v>25</v>
       </c>
       <c r="C10" s="5">
-        <v>565</v>
+        <v>464</v>
       </c>
       <c r="D10" s="5">
-        <v>464</v>
-      </c>
-      <c r="E10" s="6"/>
+        <v>570</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="4">
+        <v>75</v>
+      </c>
+      <c r="D11" s="4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="4">
-        <v>89</v>
-      </c>
-      <c r="D11" s="4">
-        <v>75</v>
-      </c>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="16"/>
@@ -1649,11 +1642,11 @@
       <c r="D17" s="16"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="15"/>
+      <c r="B19" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="14"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
@@ -1669,7 +1662,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="5">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="D21" s="5"/>
     </row>
@@ -1687,7 +1680,7 @@
         <v>29</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D23" s="5"/>
     </row>
@@ -1696,7 +1689,7 @@
         <v>33</v>
       </c>
       <c r="C24" s="5">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D24" s="5"/>
     </row>
@@ -1705,25 +1698,25 @@
         <v>23</v>
       </c>
       <c r="C25" s="5">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="D25" s="5"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="D26" s="5"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="5">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D27" s="5"/>
     </row>
@@ -1732,15 +1725,15 @@
         <v>25</v>
       </c>
       <c r="C28" s="4">
-        <v>565</v>
+        <v>570</v>
       </c>
       <c r="D28" s="5"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="17"/>
+      <c r="B29" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="15"/>
     </row>
     <row r="30" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="16"/>

</xml_diff>

<commit_message>
Added genetic selenocysteine reactions unfinished
</commit_message>
<xml_diff>
--- a/Paper/excel figures.xlsx
+++ b/Paper/excel figures.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="64">
   <si>
     <t>KO Genes</t>
   </si>
@@ -227,9 +227,6 @@
     <t>Model Top Error</t>
   </si>
   <si>
-    <t>iMR533</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -277,6 +274,9 @@
   </si>
   <si>
     <t>Table 1B. Some basic statistics for the iMR533 model.</t>
+  </si>
+  <si>
+    <t>Trans. Rxns</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -427,6 +427,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -599,11 +602,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="104118144"/>
-        <c:axId val="104119680"/>
+        <c:axId val="104445824"/>
+        <c:axId val="104447360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="104118144"/>
+        <c:axId val="104445824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -612,7 +615,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104119680"/>
+        <c:crossAx val="104447360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -620,7 +623,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104119680"/>
+        <c:axId val="104447360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -631,7 +634,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104118144"/>
+        <c:crossAx val="104445824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1480,16 +1483,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E33"/>
+  <dimension ref="A2:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D17"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="48" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -1510,7 +1514,7 @@
         <v>28</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -1546,7 +1550,7 @@
         <v>30</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -1594,24 +1598,25 @@
         <v>464</v>
       </c>
       <c r="D10" s="5">
-        <v>570</v>
+        <v>575</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="4">
         <v>75</v>
       </c>
-      <c r="D11" s="4">
-        <v>91</v>
+      <c r="D11" s="18">
+        <f>100*D10/(D8+F22)</f>
+        <v>91.414944356120827</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -1636,28 +1641,28 @@
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="14"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
         <v>27</v>
       </c>
@@ -1665,8 +1670,11 @@
         <v>534</v>
       </c>
       <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>31</v>
       </c>
@@ -1674,17 +1682,20 @@
         <v>31</v>
       </c>
       <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>33</v>
       </c>
@@ -1693,7 +1704,7 @@
       </c>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>23</v>
       </c>
@@ -1702,25 +1713,25 @@
       </c>
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="D26" s="5"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="C27" s="5">
         <v>220</v>
       </c>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>25</v>
       </c>
@@ -1729,22 +1740,22 @@
       </c>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
     </row>

</xml_diff>

<commit_message>
New model has archaeol lipid synthesis full path
</commit_message>
<xml_diff>
--- a/Paper/excel figures.xlsx
+++ b/Paper/excel figures.xlsx
@@ -10,14 +10,15 @@
     <sheet name="Growth Yield" sheetId="4" r:id="rId1"/>
     <sheet name="Knockout Validation" sheetId="1" r:id="rId2"/>
     <sheet name="General Model Stats" sheetId="2" r:id="rId3"/>
-    <sheet name="Metabolomics Figure" sheetId="3" r:id="rId4"/>
+    <sheet name="Gapfilled Subsystems" sheetId="3" r:id="rId4"/>
+    <sheet name="Generalized Subsystems" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="112">
   <si>
     <t>KO Genes</t>
   </si>
@@ -255,28 +256,172 @@
     <t>Transport/Exchange Reactions</t>
   </si>
   <si>
-    <t>58/57</t>
-  </si>
-  <si>
     <t>Dead End Reactions</t>
   </si>
   <si>
     <t>% Reactions Associated with Genes (non-exchange)</t>
   </si>
   <si>
-    <t>iMR534</t>
-  </si>
-  <si>
-    <t>650/52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Table 1A. A comparison between iMR533 and iMM518 indicates that our model covers slightly more of the genome, including over 100 more gene-associated reactions. Both models include approximately the same number of reactions, but our model has approximately 100 more internal metabolites and dead end metabolites. Though this represent the portion of metabolism that cannot carry flux, all of our model's dead end metabolites are part of gene-associated reactions and thus represent promising avenues for future model expansion. </t>
-  </si>
-  <si>
-    <t>Table 1B. Some basic statistics for the iMR533 model.</t>
-  </si>
-  <si>
     <t>Trans. Rxns</t>
+  </si>
+  <si>
+    <t>Coenzyme F430 Biosynthesis</t>
+  </si>
+  <si>
+    <t>Coenzyme B Biosynthesis</t>
+  </si>
+  <si>
+    <t>Purine Conversions</t>
+  </si>
+  <si>
+    <t>Fatty Acid Biosynthesis</t>
+  </si>
+  <si>
+    <t>Coenzyme B12 Biosynthesis</t>
+  </si>
+  <si>
+    <t>Lysine Biosynthesis DAP Pathway</t>
+  </si>
+  <si>
+    <t>Thiamin Biosynthesis</t>
+  </si>
+  <si>
+    <t>NAD/NADP Cofactor Biosynthesis</t>
+  </si>
+  <si>
+    <t>Menaquinone and Phylloquinone Biosynthesis</t>
+  </si>
+  <si>
+    <t>Chorismate Synthesis; Phenylalanine Synthesis</t>
+  </si>
+  <si>
+    <t>Isoprenoid Biosynthesis; Archaeal Lipids</t>
+  </si>
+  <si>
+    <t>Branched Chain Amino Acid Biosynthesis</t>
+  </si>
+  <si>
+    <t>Threonine Degradation; Glycine Biosynthesis</t>
+  </si>
+  <si>
+    <t>Glycolate, Glyoxylate Interconversions</t>
+  </si>
+  <si>
+    <t>Threonine Degradation; Arginine and Ornithine Degradation</t>
+  </si>
+  <si>
+    <t>Polyamine Metabolism; Arginine and Ornithine Degradation</t>
+  </si>
+  <si>
+    <t>Ubiquionine Biosynthesis</t>
+  </si>
+  <si>
+    <t>Glutathione: Biosynthesis and gamma-Glutamyl Cycle</t>
+  </si>
+  <si>
+    <t>Serine-Glyoxylate Cycle</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Pyruvate Metabolism II: Acetyl-CoA, Acetogenesis from Pyruvate</t>
+  </si>
+  <si>
+    <t>Inorganic Sulfur Assimilation</t>
+  </si>
+  <si>
+    <t>Riboflavin, FMN, and FAD Metabolism</t>
+  </si>
+  <si>
+    <t>Non-Growth Associated Maintenance</t>
+  </si>
+  <si>
+    <t>Methanofuran Biosynthesis</t>
+  </si>
+  <si>
+    <t>Methylglyoxal Metabolism</t>
+  </si>
+  <si>
+    <t>Coenzyme F420 Biosynthesis</t>
+  </si>
+  <si>
+    <t>Coenzyme A Biosynthesis</t>
+  </si>
+  <si>
+    <t>Archaellin Synthesis</t>
+  </si>
+  <si>
+    <t>De Novo Purine Biosynthesis</t>
+  </si>
+  <si>
+    <t>Sulfur Assimilation</t>
+  </si>
+  <si>
+    <t>Coenzyme M Biosynthesis</t>
+  </si>
+  <si>
+    <t>Tetrahydromethanopterin Biosynthesis</t>
+  </si>
+  <si>
+    <t>Subsystem name</t>
+  </si>
+  <si>
+    <t>Freq.</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>**classifyGapRxns(model)</t>
+  </si>
+  <si>
+    <t>Selenocysteine metabolism</t>
+  </si>
+  <si>
+    <t>Custom Subsystem</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Unique Coenzyme Syntheses</t>
+  </si>
+  <si>
+    <t>Vitamin and Cofactor Synthesis</t>
+  </si>
+  <si>
+    <t>Amino Acid Biosynthesis/Degradation</t>
+  </si>
+  <si>
+    <t>Quinone Metabolism</t>
+  </si>
+  <si>
+    <t>Nucelotide Conversions</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Archaeal Lipids and Carbohydrates</t>
+  </si>
+  <si>
+    <t>665/53</t>
+  </si>
+  <si>
+    <t>iMR544</t>
+  </si>
+  <si>
+    <t>59/59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 1A. A comparison between iMR544 and iMM518 indicates that our model covers slightly more of the genome, including over 100 more gene-associated reactions. Both models include approximately the same number of reactions, but our model has approximately 100 more internal metabolites and dead end metabolites. Though this represent the portion of metabolism that cannot carry flux, all of our model's dead end metabolites are part of gene-associated reactions and thus represent promising avenues for future model expansion. </t>
+  </si>
+  <si>
+    <t>Table 1B. Some basic statistics for the iMR544 model.</t>
   </si>
 </sst>
 </file>
@@ -420,6 +565,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -427,9 +575,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -602,11 +747,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="104445824"/>
-        <c:axId val="104447360"/>
+        <c:axId val="53880704"/>
+        <c:axId val="53882240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="104445824"/>
+        <c:axId val="53880704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -615,7 +760,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104447360"/>
+        <c:crossAx val="53882240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -623,7 +768,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104447360"/>
+        <c:axId val="53882240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -634,13 +779,397 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104445824"/>
+        <c:crossAx val="53880704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Gapfilled Subsystems'!$M$2:$M$33</c:f>
+              <c:strCache>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>Tetrahydromethanopterin Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Coenzyme M Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sulfur Assimilation</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>De Novo Purine Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Archaellin Synthesis</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Coenzyme A Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Coenzyme F420 Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Methylglyoxal Metabolism</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Methanofuran Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Non-Growth Associated Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Riboflavin, FMN, and FAD Metabolism</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Inorganic Sulfur Assimilation</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Pyruvate Metabolism II: Acetyl-CoA, Acetogenesis from Pyruvate</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>None</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Serine-Glyoxylate Cycle</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Glutathione: Biosynthesis and gamma-Glutamyl Cycle</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Ubiquionine Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Polyamine Metabolism; Arginine and Ornithine Degradation</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Threonine Degradation; Arginine and Ornithine Degradation</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Glycolate, Glyoxylate Interconversions</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Threonine Degradation; Glycine Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Branched Chain Amino Acid Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Isoprenoid Biosynthesis; Archaeal Lipids</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Chorismate Synthesis; Phenylalanine Synthesis</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Menaquinone and Phylloquinone Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>NAD/NADP Cofactor Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Thiamin Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Lysine Biosynthesis DAP Pathway</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Coenzyme B12 Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Fatty Acid Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Selenocysteine metabolism</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Purine Conversions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Gapfilled Subsystems'!$N$2:$N$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Generalized Subsystems'!$G$2:$G$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Unique Coenzyme Syntheses</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Vitamin and Cofactor Synthesis</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Amino Acid Biosynthesis/Degradation</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quinone Metabolism</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Sulfur Assimilation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>None</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Archaeal Lipids and Carbohydrates</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Nucelotide Conversions</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Other</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Generalized Subsystems'!$H$2:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -669,6 +1198,76 @@
       <xdr:colOff>308610</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>102870</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>133351</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>134021</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1486,7 +2085,7 @@
   <dimension ref="A2:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1498,11 +2097,11 @@
   <sheetData>
     <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -1514,7 +2113,7 @@
         <v>28</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -1526,7 +2125,7 @@
         <v>518</v>
       </c>
       <c r="D4" s="5">
-        <v>534</v>
+        <v>544</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -1538,7 +2137,7 @@
         <v>30</v>
       </c>
       <c r="D5" s="5">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -1550,7 +2149,7 @@
         <v>30</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -1562,7 +2161,7 @@
         <v>163</v>
       </c>
       <c r="D7" s="5">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
@@ -1574,7 +2173,7 @@
         <v>570</v>
       </c>
       <c r="D8" s="5">
-        <v>571</v>
+        <v>586</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1586,7 +2185,7 @@
         <v>49</v>
       </c>
       <c r="D9" s="5">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1598,59 +2197,58 @@
         <v>464</v>
       </c>
       <c r="D10" s="5">
-        <v>575</v>
+        <v>590</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="4">
         <v>75</v>
       </c>
-      <c r="D11" s="18">
-        <f>100*D10/(D8+F22)</f>
-        <v>91.414944356120827</v>
+      <c r="D11" s="15">
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
+      <c r="B12" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="17"/>
+      <c r="C19" s="18"/>
       <c r="D19" s="14"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -1658,7 +2256,7 @@
         <v>26</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
       <c r="D20" s="5"/>
     </row>
@@ -1667,11 +2265,11 @@
         <v>27</v>
       </c>
       <c r="C21" s="5">
-        <v>534</v>
+        <v>544</v>
       </c>
       <c r="D21" s="5"/>
       <c r="F21" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -1679,11 +2277,11 @@
         <v>31</v>
       </c>
       <c r="C22" s="5">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D22" s="5"/>
       <c r="F22">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
@@ -1691,7 +2289,7 @@
         <v>29</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>60</v>
+        <v>107</v>
       </c>
       <c r="D23" s="5"/>
     </row>
@@ -1700,7 +2298,7 @@
         <v>33</v>
       </c>
       <c r="C24" s="5">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D24" s="5"/>
     </row>
@@ -1709,7 +2307,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="5">
-        <v>571</v>
+        <v>586</v>
       </c>
       <c r="D25" s="5"/>
     </row>
@@ -1718,16 +2316,16 @@
         <v>55</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>56</v>
+        <v>109</v>
       </c>
       <c r="D26" s="5"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="5">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D27" s="5"/>
     </row>
@@ -1736,32 +2334,32 @@
         <v>25</v>
       </c>
       <c r="C28" s="4">
-        <v>570</v>
+        <v>590</v>
       </c>
       <c r="D28" s="5"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="15"/>
+      <c r="B29" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="16"/>
     </row>
     <row r="30" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
       <c r="D30" s="5"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1777,14 +2375,983 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:O40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="13" max="13" width="59.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>92</v>
+      </c>
+      <c r="N1" t="s">
+        <v>93</v>
+      </c>
+      <c r="O1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>91</v>
+      </c>
+      <c r="N2">
+        <v>9</v>
+      </c>
+      <c r="O2">
+        <v>10.588235294117647</v>
+      </c>
+    </row>
+    <row r="3" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>90</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="4" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>89</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="5" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>88</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="6" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>87</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="7" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>86</v>
+      </c>
+      <c r="N7">
+        <v>2</v>
+      </c>
+      <c r="O7">
+        <v>2.3529411764705883</v>
+      </c>
+    </row>
+    <row r="8" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>85</v>
+      </c>
+      <c r="N8">
+        <v>2</v>
+      </c>
+      <c r="O8">
+        <v>2.3529411764705883</v>
+      </c>
+    </row>
+    <row r="9" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>84</v>
+      </c>
+      <c r="N9">
+        <v>4</v>
+      </c>
+      <c r="O9">
+        <v>4.7058823529411766</v>
+      </c>
+    </row>
+    <row r="10" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>83</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="11" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>82</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="12" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>81</v>
+      </c>
+      <c r="N12">
+        <v>2</v>
+      </c>
+      <c r="O12">
+        <v>2.3529411764705883</v>
+      </c>
+    </row>
+    <row r="13" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M13" t="s">
+        <v>80</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="14" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>79</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="15" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>78</v>
+      </c>
+      <c r="N15">
+        <v>15</v>
+      </c>
+      <c r="O15">
+        <v>17.647058823529413</v>
+      </c>
+    </row>
+    <row r="16" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>77</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="17" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>76</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="18" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>75</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="19" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>74</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="20" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>73</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="21" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>72</v>
+      </c>
+      <c r="N21">
+        <v>2</v>
+      </c>
+      <c r="O21">
+        <v>2.3529411764705883</v>
+      </c>
+    </row>
+    <row r="22" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>71</v>
+      </c>
+      <c r="N22">
+        <v>2</v>
+      </c>
+      <c r="O22">
+        <v>2.3529411764705883</v>
+      </c>
+    </row>
+    <row r="23" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>70</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="24" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>69</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="25" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>68</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="26" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M26" t="s">
+        <v>67</v>
+      </c>
+      <c r="N26">
+        <v>7</v>
+      </c>
+      <c r="O26">
+        <v>8.235294117647058</v>
+      </c>
+    </row>
+    <row r="27" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M27" t="s">
+        <v>66</v>
+      </c>
+      <c r="N27">
+        <v>2</v>
+      </c>
+      <c r="O27">
+        <v>2.3529411764705883</v>
+      </c>
+    </row>
+    <row r="28" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M28" t="s">
+        <v>65</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="29" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M29" t="s">
+        <v>64</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="30" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M30" t="s">
+        <v>63</v>
+      </c>
+      <c r="N30">
+        <v>4</v>
+      </c>
+      <c r="O30">
+        <v>4.7058823529411766</v>
+      </c>
+    </row>
+    <row r="31" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M31" t="s">
+        <v>62</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="32" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M32" t="s">
+        <v>97</v>
+      </c>
+      <c r="N32">
+        <v>2</v>
+      </c>
+      <c r="O32">
+        <v>2.3529411764705883</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M33" t="s">
+        <v>61</v>
+      </c>
+      <c r="N33">
+        <v>2</v>
+      </c>
+      <c r="O33">
+        <v>2.3529411764705883</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M34" t="s">
+        <v>60</v>
+      </c>
+      <c r="N34">
+        <v>6</v>
+      </c>
+      <c r="O34">
+        <v>7.0588235294117645</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M35" t="s">
+        <v>59</v>
+      </c>
+      <c r="N35">
+        <v>5</v>
+      </c>
+      <c r="O35">
+        <v>5.882352941176471</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="M37" t="s">
+        <v>95</v>
+      </c>
+      <c r="N37">
+        <f>SUM(N2:N35)</f>
+        <v>85</v>
+      </c>
+      <c r="O37">
+        <f>SUM(O2:O35)</f>
+        <v>100.00000000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="G1:P37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="59.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <f>O2+O3+O8+O10+O34+O35</f>
+        <v>24</v>
+      </c>
+      <c r="I2" s="13">
+        <f>H2/85</f>
+        <v>0.28235294117647058</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="O2" s="2">
+        <v>9</v>
+      </c>
+      <c r="P2" s="2">
+        <v>10.588235294117647</v>
+      </c>
+    </row>
+    <row r="3" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3">
+        <f>O7+O30+O28+O27+O12</f>
+        <v>11</v>
+      </c>
+      <c r="I3" s="13">
+        <f t="shared" ref="I3:I20" si="0">H3/85</f>
+        <v>0.12941176470588237</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1</v>
+      </c>
+      <c r="P3" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="4" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4">
+        <f>O20+O22+O23+O25+O29+O32+O9</f>
+        <v>12</v>
+      </c>
+      <c r="I4" s="13">
+        <f t="shared" si="0"/>
+        <v>0.14117647058823529</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="O4" s="2">
+        <v>1</v>
+      </c>
+      <c r="P4" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="5" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5">
+        <f>O18+O26</f>
+        <v>8</v>
+      </c>
+      <c r="I5" s="13">
+        <f t="shared" si="0"/>
+        <v>9.4117647058823528E-2</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O5" s="2">
+        <v>1</v>
+      </c>
+      <c r="P5" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="6" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6">
+        <f>SUM(O4,O13)</f>
+        <v>2</v>
+      </c>
+      <c r="I6" s="13">
+        <f t="shared" si="0"/>
+        <v>2.3529411764705882E-2</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="O6" s="2">
+        <v>1</v>
+      </c>
+      <c r="P6" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="7" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7">
+        <f>O15</f>
+        <v>15</v>
+      </c>
+      <c r="I7" s="13">
+        <f t="shared" si="0"/>
+        <v>0.17647058823529413</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="O7" s="2">
+        <v>2</v>
+      </c>
+      <c r="P7" s="2">
+        <v>2.3529411764705883</v>
+      </c>
+    </row>
+    <row r="8" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8">
+        <f>SUM(O6,O24)</f>
+        <v>2</v>
+      </c>
+      <c r="I8" s="13">
+        <f t="shared" si="0"/>
+        <v>2.3529411764705882E-2</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="O8" s="2">
+        <v>2</v>
+      </c>
+      <c r="P8" s="2">
+        <v>2.3529411764705883</v>
+      </c>
+    </row>
+    <row r="9" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9">
+        <f>SUM(O33,O5)</f>
+        <v>3</v>
+      </c>
+      <c r="I9" s="13">
+        <f t="shared" si="0"/>
+        <v>3.5294117647058823E-2</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O9" s="2">
+        <v>4</v>
+      </c>
+      <c r="P9" s="2">
+        <v>4.7058823529411766</v>
+      </c>
+    </row>
+    <row r="10" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10">
+        <f>SUM(O11,O14,O16,O17,O19,O21,O31)</f>
+        <v>8</v>
+      </c>
+      <c r="I10" s="13">
+        <f t="shared" si="0"/>
+        <v>9.4117647058823528E-2</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="O10" s="2">
+        <v>1</v>
+      </c>
+      <c r="P10" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="11" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="I11" s="13"/>
+      <c r="N11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O11" s="2">
+        <v>1</v>
+      </c>
+      <c r="P11" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="12" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="I12" s="13"/>
+      <c r="N12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O12" s="2">
+        <v>2</v>
+      </c>
+      <c r="P12" s="2">
+        <v>2.3529411764705883</v>
+      </c>
+    </row>
+    <row r="13" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="I13" s="13"/>
+      <c r="N13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O13" s="2">
+        <v>1</v>
+      </c>
+      <c r="P13" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="14" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="I14" s="13"/>
+      <c r="N14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="O14" s="2">
+        <v>1</v>
+      </c>
+      <c r="P14" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="15" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="I15" s="13"/>
+      <c r="N15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="O15" s="2">
+        <v>15</v>
+      </c>
+      <c r="P15" s="2">
+        <v>17.647058823529413</v>
+      </c>
+    </row>
+    <row r="16" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="I16" s="13"/>
+      <c r="N16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="O16" s="2">
+        <v>1</v>
+      </c>
+      <c r="P16" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="17" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I17" s="13"/>
+      <c r="N17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="O17" s="2">
+        <v>1</v>
+      </c>
+      <c r="P17" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="18" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I18" s="13"/>
+      <c r="N18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="O18" s="2">
+        <v>1</v>
+      </c>
+      <c r="P18" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="19" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I19" s="13"/>
+      <c r="N19" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="O19" s="2">
+        <v>1</v>
+      </c>
+      <c r="P19" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="20" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I20" s="13"/>
+      <c r="N20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O20" s="2">
+        <v>1</v>
+      </c>
+      <c r="P20" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="21" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I21" s="13"/>
+      <c r="N21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O21" s="2">
+        <v>2</v>
+      </c>
+      <c r="P21" s="2">
+        <v>2.3529411764705883</v>
+      </c>
+    </row>
+    <row r="22" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I22" s="13"/>
+      <c r="N22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O22" s="2">
+        <v>2</v>
+      </c>
+      <c r="P22" s="2">
+        <v>2.3529411764705883</v>
+      </c>
+    </row>
+    <row r="23" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I23" s="13"/>
+      <c r="N23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O23" s="2">
+        <v>1</v>
+      </c>
+      <c r="P23" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="24" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I24" s="13"/>
+      <c r="N24" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O24" s="2">
+        <v>1</v>
+      </c>
+      <c r="P24" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="25" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I25" s="13"/>
+      <c r="N25" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="O25" s="2">
+        <v>1</v>
+      </c>
+      <c r="P25" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="26" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I26" s="13"/>
+      <c r="N26" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O26" s="2">
+        <v>7</v>
+      </c>
+      <c r="P26" s="2">
+        <v>8.235294117647058</v>
+      </c>
+    </row>
+    <row r="27" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I27" s="13"/>
+      <c r="N27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O27" s="2">
+        <v>2</v>
+      </c>
+      <c r="P27" s="2">
+        <v>2.3529411764705883</v>
+      </c>
+    </row>
+    <row r="28" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I28" s="13"/>
+      <c r="N28" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O28" s="2">
+        <v>1</v>
+      </c>
+      <c r="P28" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="29" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I29" s="13"/>
+      <c r="N29" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O29" s="2">
+        <v>1</v>
+      </c>
+      <c r="P29" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="30" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I30" s="13"/>
+      <c r="N30" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O30" s="2">
+        <v>4</v>
+      </c>
+      <c r="P30" s="2">
+        <v>4.7058823529411766</v>
+      </c>
+    </row>
+    <row r="31" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I31" s="13"/>
+      <c r="N31" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="O31" s="2">
+        <v>1</v>
+      </c>
+      <c r="P31" s="2">
+        <v>1.1764705882352942</v>
+      </c>
+    </row>
+    <row r="32" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I32" s="13"/>
+      <c r="N32" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="O32" s="2">
+        <v>2</v>
+      </c>
+      <c r="P32" s="2">
+        <v>2.3529411764705883</v>
+      </c>
+    </row>
+    <row r="33" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="I33" s="13"/>
+      <c r="N33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O33" s="2">
+        <v>2</v>
+      </c>
+      <c r="P33" s="2">
+        <v>2.3529411764705883</v>
+      </c>
+    </row>
+    <row r="34" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="I34" s="13"/>
+      <c r="N34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="O34" s="2">
+        <v>6</v>
+      </c>
+      <c r="P34" s="2">
+        <v>7.0588235294117645</v>
+      </c>
+    </row>
+    <row r="35" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="I35" s="13"/>
+      <c r="N35" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="O35" s="2">
+        <v>5</v>
+      </c>
+      <c r="P35" s="2">
+        <v>5.882352941176471</v>
+      </c>
+    </row>
+    <row r="37" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>99</v>
+      </c>
+      <c r="H37">
+        <f>SUM(H2:H35)</f>
+        <v>85</v>
+      </c>
+      <c r="I37" s="13">
+        <f>SUM(I2:I35)</f>
+        <v>1</v>
+      </c>
+      <c r="N37" t="s">
+        <v>95</v>
+      </c>
+      <c r="O37">
+        <f>SUM(O2:O35)</f>
+        <v>85</v>
+      </c>
+      <c r="P37">
+        <f>SUM(P2:P35)</f>
+        <v>100.00000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
GAPOR switching and paper edits
</commit_message>
<xml_diff>
--- a/Paper/excel figures.xlsx
+++ b/Paper/excel figures.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="120">
   <si>
     <t>Formate</t>
   </si>
@@ -425,6 +425,27 @@
   </si>
   <si>
     <t>9 of 10</t>
+  </si>
+  <si>
+    <t>Figure 2. GAPOR turned off</t>
+  </si>
+  <si>
+    <t>27 of 30</t>
+  </si>
+  <si>
+    <t>Figure 2. GAPOR on, ACS irreversible</t>
+  </si>
+  <si>
+    <t>Figure 2. GAPOR turned off, ACS irreversible</t>
+  </si>
+  <si>
+    <t>Figure 2. Switching GAPOR at the end</t>
+  </si>
+  <si>
+    <t>Figure 2. Switching GAPOR at the end, ACS irreversible</t>
+  </si>
+  <si>
+    <t>29 of 30</t>
   </si>
 </sst>
 </file>
@@ -930,11 +951,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="104522496"/>
-        <c:axId val="104524032"/>
+        <c:axId val="83620608"/>
+        <c:axId val="83622144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="104522496"/>
+        <c:axId val="83620608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -943,7 +964,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104524032"/>
+        <c:crossAx val="83622144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -951,7 +972,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104524032"/>
+        <c:axId val="83622144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -962,7 +983,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104522496"/>
+        <c:crossAx val="83620608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2322,19 +2343,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H22"/>
+  <dimension ref="B1:R69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="5" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:18" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B1" s="23" t="s">
         <v>110</v>
       </c>
@@ -2350,8 +2374,23 @@
       <c r="F1" s="25" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L1" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="M1" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
         <v>3</v>
       </c>
@@ -2367,8 +2406,23 @@
       <c r="F2" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
         <v>4</v>
       </c>
@@ -2384,8 +2438,23 @@
       <c r="F3" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
         <v>5</v>
       </c>
@@ -2401,8 +2470,23 @@
       <c r="F4" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L4" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
         <v>6</v>
       </c>
@@ -2418,8 +2502,23 @@
       <c r="F5" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
         <v>7</v>
       </c>
@@ -2435,8 +2534,23 @@
       <c r="F6" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L6" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="17" t="s">
         <v>18</v>
       </c>
@@ -2452,8 +2566,23 @@
       <c r="F7" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L7" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
         <v>44</v>
       </c>
@@ -2469,8 +2598,23 @@
       <c r="F8" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L8" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P8" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="17" t="s">
         <v>8</v>
       </c>
@@ -2486,8 +2630,23 @@
       <c r="F9" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L9" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="17" t="s">
         <v>9</v>
       </c>
@@ -2503,8 +2662,23 @@
       <c r="F10" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L10" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
         <v>10</v>
       </c>
@@ -2520,8 +2694,23 @@
       <c r="F11" s="13" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L11" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N11" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P11" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
         <v>11</v>
       </c>
@@ -2537,8 +2726,23 @@
       <c r="F12" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L12" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P12" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
         <v>12</v>
       </c>
@@ -2554,8 +2758,23 @@
       <c r="F13" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L13" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P13" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
         <v>13</v>
       </c>
@@ -2571,8 +2790,23 @@
       <c r="F14" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L14" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O14" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P14" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
         <v>14</v>
       </c>
@@ -2588,8 +2822,23 @@
       <c r="F15" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L15" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="P15" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
         <v>15</v>
       </c>
@@ -2608,8 +2857,26 @@
       <c r="H16" s="6" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="L16" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N16" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="O16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="P16" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="R16" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
         <v>17</v>
       </c>
@@ -2628,8 +2895,26 @@
       <c r="H17">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="L17" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P17" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="R17">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" ht="18" x14ac:dyDescent="0.35">
       <c r="B18" s="17" t="s">
         <v>45</v>
       </c>
@@ -2646,8 +2931,24 @@
         <v>33</v>
       </c>
       <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="L18" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="M18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N18" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q18" s="6"/>
+    </row>
+    <row r="19" spans="2:18" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="17" t="s">
         <v>46</v>
       </c>
@@ -2666,8 +2967,26 @@
       <c r="G19" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="L19" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="M19" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N19" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P19" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q19" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
         <v>35</v>
       </c>
@@ -2689,10 +3008,1394 @@
       <c r="H20" s="7">
         <v>0.86699999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="L20" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="M20" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="N20" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="O20" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="P20" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q20" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="R20" s="7">
+        <v>0.86699999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>32</v>
+      </c>
+      <c r="L22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B25" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L25" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="M25" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="N25" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="O25" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="P25" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B26" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="M26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O26" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P26" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B27" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L27" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="M27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O27" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P27" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B28" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L28" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="M28" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N28" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O28" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P28" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B29" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L29" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="M29" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N29" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O29" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P29" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B30" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L30" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="M30" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O30" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P30" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B31" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L31" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="M31" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="N31" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O31" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P31" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B32" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L32" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M32" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N32" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O32" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P32" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B33" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L33" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N33" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O33" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P33" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B34" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L34" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N34" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O34" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P34" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B35" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="L35" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N35" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P35" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B36" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L36" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N36" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O36" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P36" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B37" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L37" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="M37" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N37" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="O37" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P37" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B38" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L38" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="M38" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N38" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O38" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P38" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B39" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L39" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M39" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N39" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="O39" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="P39" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B40" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L40" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M40" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N40" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="O40" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="P40" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="R40" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B41" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H41">
+        <v>0.67</v>
+      </c>
+      <c r="L41" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="M41" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N41" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O41" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P41" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="R41">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="B42" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G42" s="6"/>
+      <c r="L42" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="M42" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N42" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P42" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q42" s="6"/>
+    </row>
+    <row r="43" spans="2:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="B43" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L43" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="M43" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N43" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="O43" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P43" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q43" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B44" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H44" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="L44" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="M44" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="N44" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="O44" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="P44" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q44" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="R44" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>113</v>
+      </c>
+      <c r="L46" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B48" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="F48" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="L48" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="M48" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="N48" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="O48" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="P48" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B49" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L49" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="M49" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N49" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O49" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P49" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B50" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L50" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="M50" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N50" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O50" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P50" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B51" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L51" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="M51" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N51" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O51" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P51" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B52" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L52" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="M52" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N52" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O52" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P52" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B53" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L53" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="M53" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N53" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O53" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P53" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B54" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L54" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="M54" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="N54" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O54" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P54" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B55" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F55" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L55" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M55" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N55" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O55" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P55" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B56" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L56" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="M56" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N56" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O56" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P56" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B57" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F57" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L57" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N57" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O57" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P57" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B58" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="L58" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="M58" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N58" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="O58" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P58" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B59" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L59" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="M59" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N59" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O59" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P59" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B60" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L60" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="M60" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N60" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="O60" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P60" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B61" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L61" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="M61" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N61" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O61" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P61" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B62" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F62" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="L62" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M62" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N62" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="O62" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="P62" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B63" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F63" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L63" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M63" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="N63" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="O63" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="P63" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="R63" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B64" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F64" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H64">
+        <v>0.67</v>
+      </c>
+      <c r="L64" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="M64" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N64" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O64" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P64" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="R64">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="65" spans="2:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="B65" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F65" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G65" s="6"/>
+      <c r="L65" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="M65" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N65" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O65" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P65" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q65" s="6"/>
+    </row>
+    <row r="66" spans="2:18" ht="18" x14ac:dyDescent="0.35">
+      <c r="B66" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L66" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="M66" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N66" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O66" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P66" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q66" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B67" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D67" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E67" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F67" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="H67" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="L67" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="M67" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="N67" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="O67" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="P67" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q67" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="R67" s="7">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>117</v>
+      </c>
+      <c r="L69" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major change w Eha constraint
</commit_message>
<xml_diff>
--- a/Paper/excel figures.xlsx
+++ b/Paper/excel figures.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="105" windowWidth="15570" windowHeight="8730" activeTab="5"/>
+    <workbookView xWindow="396" yWindow="108" windowWidth="15576" windowHeight="8736" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Generalized Subsystems" sheetId="5" r:id="rId1"/>
     <sheet name="Growth Yield" sheetId="4" r:id="rId2"/>
-    <sheet name="Knockout Validation" sheetId="1" r:id="rId3"/>
-    <sheet name="General Model Stats" sheetId="2" r:id="rId4"/>
-    <sheet name="Gapfilled Subsystems" sheetId="3" r:id="rId5"/>
-    <sheet name="LOOCV Growth Rates" sheetId="6" r:id="rId6"/>
+    <sheet name="LOOCV Growth Rates" sheetId="6" r:id="rId3"/>
+    <sheet name="Full Gene KO" sheetId="7" r:id="rId4"/>
+    <sheet name="Knockout Validation" sheetId="1" r:id="rId5"/>
+    <sheet name="General Model Stats" sheetId="2" r:id="rId6"/>
+    <sheet name="Gapfilled Subsystems" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="136">
   <si>
     <t>Formate</t>
   </si>
@@ -462,6 +463,39 @@
   </si>
   <si>
     <t>MER</t>
+  </si>
+  <si>
+    <t>Cases</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>ACC</t>
+  </si>
+  <si>
+    <t>4 Instance</t>
+  </si>
+  <si>
+    <t>3 Instance</t>
+  </si>
+  <si>
+    <t>2 Instance</t>
+  </si>
+  <si>
+    <t>1 Instance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure 3: </t>
   </si>
 </sst>
 </file>
@@ -666,15 +700,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -682,6 +707,15 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -809,7 +843,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -979,11 +1012,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="104341888"/>
-        <c:axId val="104343424"/>
+        <c:axId val="110184320"/>
+        <c:axId val="110185856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="104341888"/>
+        <c:axId val="110184320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -993,7 +1026,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104343424"/>
+        <c:crossAx val="110185856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1001,7 +1034,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104343424"/>
+        <c:axId val="110185856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1012,7 +1045,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104341888"/>
+        <c:crossAx val="110184320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1051,213 +1084,97 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
-          <c:cat>
+          <c:tx>
             <c:strRef>
-              <c:f>'Gapfilled Subsystems'!$M$2:$M$33</c:f>
+              <c:f>'LOOCV Growth Rates'!$B$1</c:f>
               <c:strCache>
-                <c:ptCount val="32"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Tetrahydromethanopterin Biosynthesis</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Coenzyme M Biosynthesis</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Sulfur Assimilation</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>De Novo Purine Biosynthesis</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Archaellin Synthesis</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Coenzyme A Biosynthesis</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Coenzyme F420 Biosynthesis</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Methylglyoxal Metabolism</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Methanofuran Biosynthesis</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Non-Growth Associated Maintenance</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Riboflavin, FMN, and FAD Metabolism</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Inorganic Sulfur Assimilation</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Pyruvate Metabolism II: Acetyl-CoA, Acetogenesis from Pyruvate</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>None</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Serine-Glyoxylate Cycle</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Glutathione: Biosynthesis and gamma-Glutamyl Cycle</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Ubiquionine Biosynthesis</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Polyamine Metabolism; Arginine and Ornithine Degradation</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Threonine Degradation; Arginine and Ornithine Degradation</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Glycolate, Glyoxylate Interconversions</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Threonine Degradation; Glycine Biosynthesis</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Branched Chain Amino Acid Biosynthesis</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Isoprenoid Biosynthesis; Archaeal Lipids</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Chorismate Synthesis; Phenylalanine Synthesis</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Menaquinone and Phylloquinone Biosynthesis</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>NAD/NADP Cofactor Biosynthesis</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Thiamin Biosynthesis</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Lysine Biosynthesis DAP Pathway</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>Coenzyme B12 Biosynthesis</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Fatty Acid Biosynthesis</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Selenocysteine metabolism</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>Purine Conversions</c:v>
+                  <c:v>Measured</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
-          </c:cat>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Gapfilled Subsystems'!$N$2:$N$33</c:f>
+              <c:f>'LOOCV Growth Rates'!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="32"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>8.14E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>9.0200000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.9200000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>4.65E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>7.0499999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>4.58E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2</c:v>
+                  <c:v>6.0199999999999997E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'LOOCV Growth Rates'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Predicted</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'LOOCV Growth Rates'!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.1013</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.5599999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.5499999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.65E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.2700000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.6100000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.9499999999999997E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1270,10 +1187,68 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="109349120"/>
+        <c:axId val="109355008"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="109349120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="109355008"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="109355008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Growth</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Rate (1/h)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="109349120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -1309,12 +1284,11 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
@@ -1327,8 +1301,46 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'LOOCV Growth Rates'!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>51.727234197410638</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48.340161938759181</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44.105816683252677</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.395384527843461</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41.132831366988491</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.116969705221639</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34.869502561398797</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>'LOOCV Growth Rates'!$B$2:$B$8</c:f>
               <c:numCache>
@@ -1357,10 +1369,11 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
@@ -1373,8 +1386,47 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:val>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:noFill/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'LOOCV Growth Rates'!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>51.727234197410638</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48.340161938759181</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44.105816683252677</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.395384527843461</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41.132831366988491</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.116969705221639</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34.869502561398797</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>'LOOCV Growth Rates'!$C$2:$C$8</c:f>
               <c:numCache>
@@ -1403,7 +1455,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1413,29 +1466,47 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="106394368"/>
-        <c:axId val="106455808"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="106394368"/>
+        <c:axId val="110248704"/>
+        <c:axId val="110250624"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="110248704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="60"/>
+          <c:min val="20"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Methane Secretion Rate (mmol/gDCW/h)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106455808"/>
+        <c:crossAx val="110250624"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="106455808"/>
+        <c:axId val="110250624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1470,9 +1541,9 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106394368"/>
+        <c:crossAx val="110248704"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1509,180 +1580,454 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'LOOCV Growth Rates'!$B$1</c:f>
+              <c:f>'Full Gene KO'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Measured</c:v>
+                  <c:v>TP</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="7"/>
-            <c:spPr>
-              <a:noFill/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Full Gene KO'!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4 Instance</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 Instance</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2 Instance</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1 Instance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>'LOOCV Growth Rates'!$D$2:$D$8</c:f>
+              <c:f>'Full Gene KO'!$B$2:$B$5</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>51.727234197410638</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.340161938759181</c:v>
+                  <c:v>187</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44.105816683252677</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28.395384527843461</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41.132831366988491</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>28.116969705221639</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>34.869502561398797</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'LOOCV Growth Rates'!$B$2:$B$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>8.14E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.0200000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8.9200000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.65E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.0499999999999993E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.58E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.0199999999999997E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
+          </c:val>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'LOOCV Growth Rates'!$C$1</c:f>
+              <c:f>'Full Gene KO'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Predicted</c:v>
+                  <c:v>TN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="x"/>
-            <c:size val="7"/>
-          </c:marker>
-          <c:xVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Full Gene KO'!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4 Instance</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 Instance</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2 Instance</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1 Instance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>'LOOCV Growth Rates'!$D$2:$D$8</c:f>
+              <c:f>'Full Gene KO'!$C$2:$C$5</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>51.727234197410638</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.340161938759181</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44.105816683252677</c:v>
+                  <c:v>172</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28.395384527843461</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41.132831366988491</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>28.116969705221639</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>34.869502561398797</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Full Gene KO'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Full Gene KO'!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4 Instance</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 Instance</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2 Instance</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1 Instance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>'LOOCV Growth Rates'!$C$2:$C$8</c:f>
+              <c:f>'Full Gene KO'!$D$2:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.1013</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.5599999999999996E-2</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.5499999999999998E-2</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.65E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.2700000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.6100000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.9499999999999997E-2</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Full Gene KO'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Full Gene KO'!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4 Instance</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 Instance</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2 Instance</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1 Instance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Full Gene KO'!$E$2:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="121599488"/>
+        <c:axId val="121601024"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="121599488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="121601024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="121601024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="121599488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Full Gene KO'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ACC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Full Gene KO'!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4 Instance</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 Instance</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2 Instance</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1 Instance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Full Gene KO'!$F$2:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>64.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="180146944"/>
+        <c:axId val="180143616"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Full Gene KO'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MCC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Full Gene KO'!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4 Instance</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3 Instance</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2 Instance</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1 Instance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Full Gene KO'!$G$2:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.28299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.32300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
@@ -1693,87 +2038,336 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="109198720"/>
-        <c:axId val="107047168"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="109198720"/>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="175444736"/>
+        <c:axId val="175446272"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="175444736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Methane Secretion Rate (mmol/gDCW/h)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="107047168"/>
+        <c:crossAx val="175446272"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="107047168"/>
+        <c:axId val="175446272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Growth</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Rate (1/h)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109198720"/>
+        <c:crossAx val="175444736"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="180143616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="180146944"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="180146944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="180143616"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Gapfilled Subsystems'!$M$2:$M$33</c:f>
+              <c:strCache>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>Tetrahydromethanopterin Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Coenzyme M Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sulfur Assimilation</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>De Novo Purine Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Archaellin Synthesis</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Coenzyme A Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Coenzyme F420 Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Methylglyoxal Metabolism</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Methanofuran Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Non-Growth Associated Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Riboflavin, FMN, and FAD Metabolism</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Inorganic Sulfur Assimilation</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Pyruvate Metabolism II: Acetyl-CoA, Acetogenesis from Pyruvate</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>None</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Serine-Glyoxylate Cycle</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Glutathione: Biosynthesis and gamma-Glutamyl Cycle</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Ubiquionine Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Polyamine Metabolism; Arginine and Ornithine Degradation</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Threonine Degradation; Arginine and Ornithine Degradation</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Glycolate, Glyoxylate Interconversions</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Threonine Degradation; Glycine Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Branched Chain Amino Acid Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Isoprenoid Biosynthesis; Archaeal Lipids</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Chorismate Synthesis; Phenylalanine Synthesis</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Menaquinone and Phylloquinone Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>NAD/NADP Cofactor Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Thiamin Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Lysine Biosynthesis DAP Pathway</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Coenzyme B12 Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Fatty Acid Biosynthesis</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Selenocysteine metabolism</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Purine Conversions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Gapfilled Subsystems'!$N$2:$N$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1862,41 +2456,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>523874</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
       <xdr:row>14</xdr:row>
@@ -1950,6 +2509,106 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2251,13 +2910,13 @@
       <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="59.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="59.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="7:16" ht="15" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
         <v>95</v>
       </c>
@@ -2274,7 +2933,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="7:16" ht="15" x14ac:dyDescent="0.25">
       <c r="G2" t="s">
         <v>97</v>
       </c>
@@ -2297,7 +2956,7 @@
         <v>0.10465116279069768</v>
       </c>
     </row>
-    <row r="3" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="7:16" ht="15" x14ac:dyDescent="0.25">
       <c r="G3" t="s">
         <v>98</v>
       </c>
@@ -2320,7 +2979,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="4" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="7:16" ht="15" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
         <v>99</v>
       </c>
@@ -2334,7 +2993,7 @@
       </c>
       <c r="P4" s="6"/>
     </row>
-    <row r="5" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="7:16" ht="15" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
         <v>100</v>
       </c>
@@ -2357,7 +3016,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="6" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="7:16" ht="15" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
         <v>86</v>
       </c>
@@ -2380,7 +3039,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="7" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="7:16" ht="15" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
         <v>75</v>
       </c>
@@ -2403,7 +3062,7 @@
         <v>2.3255813953488372E-2</v>
       </c>
     </row>
-    <row r="8" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="7:16" ht="15" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
         <v>103</v>
       </c>
@@ -2426,7 +3085,7 @@
         <v>2.3255813953488372E-2</v>
       </c>
     </row>
-    <row r="9" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="7:16" ht="15" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
         <v>101</v>
       </c>
@@ -2449,7 +3108,7 @@
         <v>4.6511627906976744E-2</v>
       </c>
     </row>
-    <row r="10" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="7:16" ht="15" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
         <v>102</v>
       </c>
@@ -2472,7 +3131,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="11" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="7:16" ht="15" x14ac:dyDescent="0.25">
       <c r="I11" s="6"/>
       <c r="N11" t="s">
         <v>79</v>
@@ -2485,7 +3144,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="12" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="7:16" ht="15" x14ac:dyDescent="0.25">
       <c r="I12" s="6"/>
       <c r="N12" t="s">
         <v>78</v>
@@ -2498,7 +3157,7 @@
         <v>2.3255813953488372E-2</v>
       </c>
     </row>
-    <row r="13" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="7:16" ht="15" x14ac:dyDescent="0.25">
       <c r="I13" s="6"/>
       <c r="N13" t="s">
         <v>77</v>
@@ -2511,7 +3170,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="14" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="7:16" ht="15" x14ac:dyDescent="0.25">
       <c r="I14" s="6"/>
       <c r="N14" t="s">
         <v>76</v>
@@ -2524,7 +3183,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="15" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="7:16" ht="15" x14ac:dyDescent="0.25">
       <c r="I15" s="6"/>
       <c r="N15" t="s">
         <v>75</v>
@@ -2537,7 +3196,7 @@
         <v>0.19767441860465115</v>
       </c>
     </row>
-    <row r="16" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="7:16" ht="15" x14ac:dyDescent="0.25">
       <c r="I16" s="6"/>
       <c r="N16" t="s">
         <v>74</v>
@@ -2550,7 +3209,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="17" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:16" ht="15" x14ac:dyDescent="0.25">
       <c r="I17" s="6"/>
       <c r="N17" t="s">
         <v>73</v>
@@ -2563,7 +3222,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="18" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:16" ht="15" x14ac:dyDescent="0.25">
       <c r="I18" s="6"/>
       <c r="N18" t="s">
         <v>72</v>
@@ -2576,7 +3235,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="19" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:16" ht="15" x14ac:dyDescent="0.25">
       <c r="I19" s="6"/>
       <c r="K19">
         <f>SUM(H3,H4,H5,H6,H7)/86</f>
@@ -2593,7 +3252,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="20" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:16" ht="15" x14ac:dyDescent="0.25">
       <c r="I20" s="6"/>
       <c r="K20">
         <f>K19*86</f>
@@ -2610,7 +3269,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="21" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:16" ht="15" x14ac:dyDescent="0.25">
       <c r="I21" s="6"/>
       <c r="N21" t="s">
         <v>69</v>
@@ -2623,7 +3282,7 @@
         <v>2.3255813953488372E-2</v>
       </c>
     </row>
-    <row r="22" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="9:16" ht="15" x14ac:dyDescent="0.25">
       <c r="I22" s="6"/>
       <c r="N22" t="s">
         <v>68</v>
@@ -2636,7 +3295,7 @@
         <v>2.3255813953488372E-2</v>
       </c>
     </row>
-    <row r="23" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:16" ht="15" x14ac:dyDescent="0.25">
       <c r="I23" s="6"/>
       <c r="N23" t="s">
         <v>67</v>
@@ -2649,7 +3308,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="24" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:16" ht="15" x14ac:dyDescent="0.25">
       <c r="I24" s="6"/>
       <c r="N24" t="s">
         <v>66</v>
@@ -2662,7 +3321,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="25" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:16" ht="15" x14ac:dyDescent="0.25">
       <c r="I25" s="6"/>
       <c r="N25" t="s">
         <v>65</v>
@@ -2675,7 +3334,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="26" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:16" ht="15" x14ac:dyDescent="0.25">
       <c r="I26" s="6"/>
       <c r="N26" t="s">
         <v>64</v>
@@ -2688,7 +3347,7 @@
         <v>8.1395348837209308E-2</v>
       </c>
     </row>
-    <row r="27" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="9:16" ht="15" x14ac:dyDescent="0.25">
       <c r="I27" s="6"/>
       <c r="N27" t="s">
         <v>63</v>
@@ -2701,7 +3360,7 @@
         <v>2.3255813953488372E-2</v>
       </c>
     </row>
-    <row r="28" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:16" x14ac:dyDescent="0.3">
       <c r="I28" s="6"/>
       <c r="N28" t="s">
         <v>62</v>
@@ -2714,7 +3373,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="29" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="9:16" x14ac:dyDescent="0.3">
       <c r="I29" s="6"/>
       <c r="N29" t="s">
         <v>61</v>
@@ -2727,7 +3386,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="30" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="9:16" x14ac:dyDescent="0.3">
       <c r="I30" s="6"/>
       <c r="N30" t="s">
         <v>60</v>
@@ -2740,7 +3399,7 @@
         <v>4.6511627906976744E-2</v>
       </c>
     </row>
-    <row r="31" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="9:16" x14ac:dyDescent="0.3">
       <c r="I31" s="6"/>
       <c r="N31" t="s">
         <v>59</v>
@@ -2753,7 +3412,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="32" spans="9:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="9:16" x14ac:dyDescent="0.3">
       <c r="I32" s="6"/>
       <c r="N32" t="s">
         <v>94</v>
@@ -2766,7 +3425,7 @@
         <v>2.3255813953488372E-2</v>
       </c>
     </row>
-    <row r="33" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:16" x14ac:dyDescent="0.3">
       <c r="I33" s="6"/>
       <c r="N33" t="s">
         <v>58</v>
@@ -2779,7 +3438,7 @@
         <v>2.3255813953488372E-2</v>
       </c>
     </row>
-    <row r="34" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:16" x14ac:dyDescent="0.3">
       <c r="I34" s="6"/>
       <c r="N34" t="s">
         <v>57</v>
@@ -2792,7 +3451,7 @@
         <v>6.9767441860465115E-2</v>
       </c>
     </row>
-    <row r="35" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:16" x14ac:dyDescent="0.3">
       <c r="I35" s="6"/>
       <c r="N35" t="s">
         <v>56</v>
@@ -2805,7 +3464,7 @@
         <v>5.8139534883720929E-2</v>
       </c>
     </row>
-    <row r="37" spans="7:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:16" x14ac:dyDescent="0.3">
       <c r="G37" t="s">
         <v>96</v>
       </c>
@@ -2844,12 +3503,12 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>41</v>
       </c>
@@ -2857,7 +3516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2868,7 +3527,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -2879,7 +3538,7 @@
         <v>3.22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -2890,7 +3549,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -2903,7 +3562,7 @@
         <v>3.64</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -2916,7 +3575,7 @@
         <v>2.8000000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -2929,7 +3588,7 @@
         <v>-0.19254658385093171</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -2942,12 +3601,12 @@
         <v>-0.2857142857142857</v>
       </c>
     </row>
-    <row r="22" spans="5:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="5:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:6" x14ac:dyDescent="0.3">
       <c r="F30">
         <f>-1226.2-2077.7+2011.4+1296.8</f>
         <v>4.3000000000004093</v>
@@ -2961,23 +3620,294 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>8.14E-2</v>
+      </c>
+      <c r="C2">
+        <v>0.1013</v>
+      </c>
+      <c r="D2" s="27">
+        <v>51.727234197410638</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>9.0200000000000002E-2</v>
+      </c>
+      <c r="C3">
+        <v>8.5599999999999996E-2</v>
+      </c>
+      <c r="D3" s="27">
+        <v>48.340161938759181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>8.9200000000000002E-2</v>
+      </c>
+      <c r="C4">
+        <v>7.5499999999999998E-2</v>
+      </c>
+      <c r="D4" s="27">
+        <v>44.105816683252677</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4.65E-2</v>
+      </c>
+      <c r="C5">
+        <v>4.65E-2</v>
+      </c>
+      <c r="D5" s="27">
+        <v>28.395384527843461</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>7.0499999999999993E-2</v>
+      </c>
+      <c r="C6">
+        <v>7.2700000000000001E-2</v>
+      </c>
+      <c r="D6" s="27">
+        <v>41.132831366988491</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>4.58E-2</v>
+      </c>
+      <c r="C7">
+        <v>4.6100000000000002E-2</v>
+      </c>
+      <c r="D7" s="27">
+        <v>28.116969705221639</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>6.0199999999999997E-2</v>
+      </c>
+      <c r="C8">
+        <v>5.9499999999999997E-2</v>
+      </c>
+      <c r="D8" s="27">
+        <v>34.869502561398797</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="C2">
+        <v>146</v>
+      </c>
+      <c r="D2">
+        <v>111</v>
+      </c>
+      <c r="E2">
+        <v>81</v>
+      </c>
+      <c r="F2">
+        <v>64.3</v>
+      </c>
+      <c r="G2">
+        <v>0.28299999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3">
+        <v>187</v>
+      </c>
+      <c r="C3">
+        <v>164</v>
+      </c>
+      <c r="D3">
+        <v>124</v>
+      </c>
+      <c r="E3">
+        <v>63</v>
+      </c>
+      <c r="F3">
+        <v>65.2</v>
+      </c>
+      <c r="G3">
+        <v>0.32100000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4">
+        <v>176</v>
+      </c>
+      <c r="C4">
+        <v>172</v>
+      </c>
+      <c r="D4">
+        <v>135</v>
+      </c>
+      <c r="E4">
+        <v>55</v>
+      </c>
+      <c r="F4">
+        <v>64.7</v>
+      </c>
+      <c r="G4">
+        <v>0.32300000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5">
+        <v>151</v>
+      </c>
+      <c r="C5">
+        <v>179</v>
+      </c>
+      <c r="D5">
+        <v>160</v>
+      </c>
+      <c r="E5">
+        <v>48</v>
+      </c>
+      <c r="F5">
+        <v>61.3</v>
+      </c>
+      <c r="G5">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R69"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="5" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="5" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" customWidth="1"/>
+    <col min="17" max="17" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B1" s="22" t="s">
         <v>108</v>
       </c>
@@ -3009,7 +3939,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
@@ -3041,7 +3971,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
@@ -3073,7 +4003,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="16" t="s">
         <v>5</v>
       </c>
@@ -3105,7 +4035,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="16" t="s">
         <v>6</v>
       </c>
@@ -3137,7 +4067,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="16" t="s">
         <v>7</v>
       </c>
@@ -3169,7 +4099,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="16" t="s">
         <v>18</v>
       </c>
@@ -3201,7 +4131,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="16" t="s">
         <v>44</v>
       </c>
@@ -3233,7 +4163,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="16" t="s">
         <v>8</v>
       </c>
@@ -3265,7 +4195,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="16" t="s">
         <v>9</v>
       </c>
@@ -3297,7 +4227,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="16" t="s">
         <v>10</v>
       </c>
@@ -3329,7 +4259,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" s="16" t="s">
         <v>11</v>
       </c>
@@ -3361,7 +4291,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
         <v>12</v>
       </c>
@@ -3393,7 +4323,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B14" s="16" t="s">
         <v>13</v>
       </c>
@@ -3425,7 +4355,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B15" s="16" t="s">
         <v>14</v>
       </c>
@@ -3457,7 +4387,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B16" s="16" t="s">
         <v>15</v>
       </c>
@@ -3495,7 +4425,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B17" s="16" t="s">
         <v>17</v>
       </c>
@@ -3533,7 +4463,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="18" spans="2:18" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:18" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B18" s="16" t="s">
         <v>45</v>
       </c>
@@ -3567,7 +4497,7 @@
       </c>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="2:18" ht="18" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:18" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B19" s="16" t="s">
         <v>46</v>
       </c>
@@ -3605,7 +4535,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="17" t="s">
         <v>35</v>
       </c>
@@ -3649,7 +4579,7 @@
         <v>0.86699999999999999</v>
       </c>
     </row>
-    <row r="22" spans="2:18" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>32</v>
       </c>
@@ -3657,7 +4587,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" s="22" t="s">
         <v>108</v>
       </c>
@@ -3689,7 +4619,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B26" s="16" t="s">
         <v>3</v>
       </c>
@@ -3721,7 +4651,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B27" s="16" t="s">
         <v>4</v>
       </c>
@@ -3753,7 +4683,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B28" s="16" t="s">
         <v>5</v>
       </c>
@@ -3785,7 +4715,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B29" s="16" t="s">
         <v>6</v>
       </c>
@@ -3817,7 +4747,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B30" s="16" t="s">
         <v>7</v>
       </c>
@@ -3849,7 +4779,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B31" s="16" t="s">
         <v>18</v>
       </c>
@@ -3881,7 +4811,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B32" s="16" t="s">
         <v>44</v>
       </c>
@@ -3913,7 +4843,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B33" s="16" t="s">
         <v>8</v>
       </c>
@@ -3945,7 +4875,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B34" s="16" t="s">
         <v>9</v>
       </c>
@@ -3977,7 +4907,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B35" s="16" t="s">
         <v>10</v>
       </c>
@@ -4009,7 +4939,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B36" s="16" t="s">
         <v>11</v>
       </c>
@@ -4041,7 +4971,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B37" s="16" t="s">
         <v>12</v>
       </c>
@@ -4073,7 +5003,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B38" s="16" t="s">
         <v>13</v>
       </c>
@@ -4105,7 +5035,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B39" s="16" t="s">
         <v>14</v>
       </c>
@@ -4137,7 +5067,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B40" s="16" t="s">
         <v>15</v>
       </c>
@@ -4175,7 +5105,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B41" s="16" t="s">
         <v>17</v>
       </c>
@@ -4213,7 +5143,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="42" spans="2:18" ht="18" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:18" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B42" s="16" t="s">
         <v>45</v>
       </c>
@@ -4247,7 +5177,7 @@
       </c>
       <c r="Q42" s="5"/>
     </row>
-    <row r="43" spans="2:18" ht="18" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:18" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B43" s="16" t="s">
         <v>46</v>
       </c>
@@ -4285,7 +5215,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B44" s="17" t="s">
         <v>35</v>
       </c>
@@ -4329,7 +5259,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>111</v>
       </c>
@@ -4337,7 +5267,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B48" s="22" t="s">
         <v>108</v>
       </c>
@@ -4369,7 +5299,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B49" s="16" t="s">
         <v>3</v>
       </c>
@@ -4401,7 +5331,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B50" s="16" t="s">
         <v>4</v>
       </c>
@@ -4433,7 +5363,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B51" s="16" t="s">
         <v>5</v>
       </c>
@@ -4465,7 +5395,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B52" s="16" t="s">
         <v>6</v>
       </c>
@@ -4497,7 +5427,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B53" s="16" t="s">
         <v>7</v>
       </c>
@@ -4529,7 +5459,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B54" s="16" t="s">
         <v>18</v>
       </c>
@@ -4561,7 +5491,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B55" s="16" t="s">
         <v>44</v>
       </c>
@@ -4593,7 +5523,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B56" s="16" t="s">
         <v>8</v>
       </c>
@@ -4625,7 +5555,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B57" s="16" t="s">
         <v>9</v>
       </c>
@@ -4657,7 +5587,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B58" s="16" t="s">
         <v>10</v>
       </c>
@@ -4689,7 +5619,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B59" s="16" t="s">
         <v>11</v>
       </c>
@@ -4721,7 +5651,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B60" s="16" t="s">
         <v>12</v>
       </c>
@@ -4753,7 +5683,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B61" s="16" t="s">
         <v>13</v>
       </c>
@@ -4785,7 +5715,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B62" s="16" t="s">
         <v>14</v>
       </c>
@@ -4817,7 +5747,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B63" s="16" t="s">
         <v>15</v>
       </c>
@@ -4855,7 +5785,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B64" s="16" t="s">
         <v>17</v>
       </c>
@@ -4893,7 +5823,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="65" spans="2:18" ht="18" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:18" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B65" s="16" t="s">
         <v>45</v>
       </c>
@@ -4927,7 +5857,7 @@
       </c>
       <c r="Q65" s="5"/>
     </row>
-    <row r="66" spans="2:18" ht="18" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:18" ht="15.6" x14ac:dyDescent="0.35">
       <c r="B66" s="16" t="s">
         <v>46</v>
       </c>
@@ -4965,7 +5895,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B67" s="17" t="s">
         <v>35</v>
       </c>
@@ -5009,7 +5939,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>115</v>
       </c>
@@ -5023,7 +5953,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F37"/>
   <sheetViews>
@@ -5031,23 +5961,23 @@
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>24</v>
@@ -5059,7 +5989,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
         <v>25</v>
@@ -5071,7 +6001,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
         <v>29</v>
@@ -5083,7 +6013,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
         <v>27</v>
@@ -5095,7 +6025,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
         <v>31</v>
@@ -5107,7 +6037,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
         <v>21</v>
@@ -5122,7 +6052,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
         <v>22</v>
@@ -5134,7 +6064,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="2" t="s">
         <v>23</v>
@@ -5146,7 +6076,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
         <v>54</v>
@@ -5158,51 +6088,51 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="25" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="27" t="s">
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+    </row>
+    <row r="19" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="B19" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="27"/>
+      <c r="C19" s="28"/>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>25</v>
       </c>
@@ -5214,7 +6144,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
@@ -5226,7 +6156,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>27</v>
       </c>
@@ -5235,7 +6165,7 @@
       </c>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>31</v>
       </c>
@@ -5244,7 +6174,7 @@
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>21</v>
       </c>
@@ -5253,7 +6183,7 @@
       </c>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>52</v>
       </c>
@@ -5266,7 +6196,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
         <v>53</v>
       </c>
@@ -5275,7 +6205,7 @@
       </c>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>23</v>
       </c>
@@ -5284,36 +6214,36 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="28" t="s">
+    <row r="29" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="C29" s="28"/>
-    </row>
-    <row r="30" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
+      <c r="C29" s="25"/>
+    </row>
+    <row r="30" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36">
         <f>1/0.045</f>
         <v>22.222222222222221</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37">
         <f>1/0.09</f>
         <v>11.111111111111111</v>
@@ -5330,7 +6260,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O40"/>
   <sheetViews>
@@ -5338,12 +6268,12 @@
       <selection activeCell="M1" sqref="M1:O37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="13" max="13" width="59.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="59.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M1" t="s">
         <v>89</v>
       </c>
@@ -5354,7 +6284,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M2" t="s">
         <v>88</v>
       </c>
@@ -5366,7 +6296,7 @@
         <v>0.10465116279069768</v>
       </c>
     </row>
-    <row r="3" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M3" t="s">
         <v>87</v>
       </c>
@@ -5378,7 +6308,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="4" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M4" t="s">
         <v>86</v>
       </c>
@@ -5387,7 +6317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M5" t="s">
         <v>85</v>
       </c>
@@ -5399,7 +6329,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="6" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M6" t="s">
         <v>84</v>
       </c>
@@ -5411,7 +6341,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="7" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M7" t="s">
         <v>83</v>
       </c>
@@ -5423,7 +6353,7 @@
         <v>2.3255813953488372E-2</v>
       </c>
     </row>
-    <row r="8" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M8" t="s">
         <v>82</v>
       </c>
@@ -5435,7 +6365,7 @@
         <v>2.3255813953488372E-2</v>
       </c>
     </row>
-    <row r="9" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M9" t="s">
         <v>81</v>
       </c>
@@ -5447,7 +6377,7 @@
         <v>4.6511627906976744E-2</v>
       </c>
     </row>
-    <row r="10" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M10" t="s">
         <v>80</v>
       </c>
@@ -5459,7 +6389,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="11" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M11" t="s">
         <v>79</v>
       </c>
@@ -5471,7 +6401,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="12" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M12" t="s">
         <v>78</v>
       </c>
@@ -5483,7 +6413,7 @@
         <v>2.3255813953488372E-2</v>
       </c>
     </row>
-    <row r="13" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M13" t="s">
         <v>77</v>
       </c>
@@ -5495,7 +6425,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="14" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M14" t="s">
         <v>76</v>
       </c>
@@ -5507,7 +6437,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="15" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M15" t="s">
         <v>75</v>
       </c>
@@ -5519,7 +6449,7 @@
         <v>0.19767441860465115</v>
       </c>
     </row>
-    <row r="16" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M16" t="s">
         <v>74</v>
       </c>
@@ -5531,7 +6461,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="17" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M17" t="s">
         <v>73</v>
       </c>
@@ -5543,7 +6473,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="18" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M18" t="s">
         <v>72</v>
       </c>
@@ -5555,7 +6485,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="19" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M19" t="s">
         <v>71</v>
       </c>
@@ -5567,7 +6497,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="20" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M20" t="s">
         <v>70</v>
       </c>
@@ -5579,7 +6509,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="21" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M21" t="s">
         <v>69</v>
       </c>
@@ -5591,7 +6521,7 @@
         <v>2.3255813953488372E-2</v>
       </c>
     </row>
-    <row r="22" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M22" t="s">
         <v>68</v>
       </c>
@@ -5603,7 +6533,7 @@
         <v>2.3255813953488372E-2</v>
       </c>
     </row>
-    <row r="23" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M23" t="s">
         <v>67</v>
       </c>
@@ -5615,7 +6545,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="24" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M24" t="s">
         <v>66</v>
       </c>
@@ -5627,7 +6557,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="25" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M25" t="s">
         <v>65</v>
       </c>
@@ -5639,7 +6569,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="26" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M26" t="s">
         <v>64</v>
       </c>
@@ -5651,7 +6581,7 @@
         <v>8.1395348837209308E-2</v>
       </c>
     </row>
-    <row r="27" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="13:15" ht="15" x14ac:dyDescent="0.25">
       <c r="M27" t="s">
         <v>63</v>
       </c>
@@ -5663,7 +6593,7 @@
         <v>2.3255813953488372E-2</v>
       </c>
     </row>
-    <row r="28" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="13:15" x14ac:dyDescent="0.3">
       <c r="M28" t="s">
         <v>62</v>
       </c>
@@ -5675,7 +6605,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="29" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="13:15" x14ac:dyDescent="0.3">
       <c r="M29" t="s">
         <v>61</v>
       </c>
@@ -5687,7 +6617,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="30" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="13:15" x14ac:dyDescent="0.3">
       <c r="M30" t="s">
         <v>60</v>
       </c>
@@ -5699,7 +6629,7 @@
         <v>4.6511627906976744E-2</v>
       </c>
     </row>
-    <row r="31" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="13:15" x14ac:dyDescent="0.3">
       <c r="M31" t="s">
         <v>59</v>
       </c>
@@ -5711,7 +6641,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
     </row>
-    <row r="32" spans="13:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="13:15" x14ac:dyDescent="0.3">
       <c r="M32" t="s">
         <v>94</v>
       </c>
@@ -5723,7 +6653,7 @@
         <v>2.3255813953488372E-2</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M33" t="s">
         <v>58</v>
       </c>
@@ -5735,7 +6665,7 @@
         <v>2.3255813953488372E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M34" t="s">
         <v>57</v>
       </c>
@@ -5747,7 +6677,7 @@
         <v>6.9767441860465115E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M35" t="s">
         <v>56</v>
       </c>
@@ -5759,7 +6689,7 @@
         <v>5.8139534883720929E-2</v>
       </c>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
       <c r="M37" t="s">
         <v>92</v>
       </c>
@@ -5772,7 +6702,7 @@
         <v>1.0000000000000004</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>93</v>
       </c>
@@ -5782,136 +6712,4 @@
   <pageSetup orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>8.14E-2</v>
-      </c>
-      <c r="C2">
-        <v>0.1013</v>
-      </c>
-      <c r="D2" s="30">
-        <v>51.727234197410638</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>9.0200000000000002E-2</v>
-      </c>
-      <c r="C3">
-        <v>8.5599999999999996E-2</v>
-      </c>
-      <c r="D3" s="30">
-        <v>48.340161938759181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>8.9200000000000002E-2</v>
-      </c>
-      <c r="C4">
-        <v>7.5499999999999998E-2</v>
-      </c>
-      <c r="D4" s="30">
-        <v>44.105816683252677</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>4.65E-2</v>
-      </c>
-      <c r="C5">
-        <v>4.65E-2</v>
-      </c>
-      <c r="D5" s="30">
-        <v>28.395384527843461</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>7.0499999999999993E-2</v>
-      </c>
-      <c r="C6">
-        <v>7.2700000000000001E-2</v>
-      </c>
-      <c r="D6" s="30">
-        <v>41.132831366988491</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>4.58E-2</v>
-      </c>
-      <c r="C7">
-        <v>4.6100000000000002E-2</v>
-      </c>
-      <c r="D7" s="30">
-        <v>28.116969705221639</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>6.0199999999999997E-2</v>
-      </c>
-      <c r="C8">
-        <v>5.9499999999999997E-2</v>
-      </c>
-      <c r="D8" s="30">
-        <v>34.869502561398797</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated KO Panel Code
</commit_message>
<xml_diff>
--- a/Paper/excel figures.xlsx
+++ b/Paper/excel figures.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="105" windowWidth="15570" windowHeight="8730" activeTab="3"/>
+    <workbookView xWindow="390" yWindow="105" windowWidth="15570" windowHeight="8730" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Model Stats" sheetId="2" r:id="rId1"/>
     <sheet name="Generalized Subsystems" sheetId="5" r:id="rId2"/>
     <sheet name="LOOCV Growth Rates" sheetId="6" r:id="rId3"/>
-    <sheet name="Full Gene KO" sheetId="7" r:id="rId4"/>
-    <sheet name="Knockout Validation" sheetId="1" r:id="rId5"/>
+    <sheet name="Knockout Validation" sheetId="1" r:id="rId4"/>
+    <sheet name="Full Gene KO" sheetId="7" r:id="rId5"/>
     <sheet name="Growth Yield" sheetId="4" r:id="rId6"/>
     <sheet name="Gapfilled Subsystems" sheetId="3" r:id="rId7"/>
   </sheets>
@@ -140,9 +140,6 @@
     <t>Dead End Metabolites</t>
   </si>
   <si>
-    <t>Figure 2. Knockout lethality predictions from FBA and agreement with experimental results</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -459,16 +456,19 @@
     <t>1 Instance</t>
   </si>
   <si>
-    <t>Figure 3B: Accuracy and Matthews Correlation Coefficient (MCC) o</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Figure 3A: Full results of comparing model predictions of gene essentiality with essentiality index (EI). The 4 "instances" denote the cutoff for how many of the 4 libraries gave an "essential" prediction for a given gene; thus a "4 instance" essential gene was essential in all 4 libraries, a "1 instance" essential gene was essential in at least 1 library. Essentiality predictions were classified as "positive" in relation </t>
-  </si>
-  <si>
     <t>iMR540</t>
   </si>
   <si>
     <t>10 of 10</t>
+  </si>
+  <si>
+    <t>Figure 3. Knockout lethality predictions from FBA and agreement with experimental results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figure S1: Full results of comparing model predictions of gene essentiality with essentiality index (EI). The 4 "instances" denote the cutoff for how many of the 4 libraries gave an "essential" prediction for a given gene; thus a "4 instance" essential gene was essential in all 4 libraries, a "1 instance" essential gene was essential in at least 1 library. Essentiality predictions were classified as "positive" in relation </t>
+  </si>
+  <si>
+    <t>Figure S2: Accuracy and Matthews Correlation Coefficient (MCC) o</t>
   </si>
 </sst>
 </file>
@@ -686,6 +686,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -701,7 +702,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -965,11 +965,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="40941440"/>
-        <c:axId val="40942976"/>
+        <c:axId val="83475456"/>
+        <c:axId val="83485440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="40941440"/>
+        <c:axId val="83475456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -978,7 +978,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40942976"/>
+        <c:crossAx val="83485440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -986,7 +986,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40942976"/>
+        <c:axId val="83485440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1021,7 +1021,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40941440"/>
+        <c:crossAx val="83475456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1242,11 +1242,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="41267200"/>
-        <c:axId val="41269504"/>
+        <c:axId val="93402240"/>
+        <c:axId val="93404544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="41267200"/>
+        <c:axId val="93402240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -1277,12 +1277,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41269504"/>
+        <c:crossAx val="93404544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="41269504"/>
+        <c:axId val="93404544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1317,7 +1317,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41267200"/>
+        <c:crossAx val="93402240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1597,11 +1597,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="41305216"/>
-        <c:axId val="41306752"/>
+        <c:axId val="94734592"/>
+        <c:axId val="94744576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="41305216"/>
+        <c:axId val="94734592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1611,7 +1611,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41306752"/>
+        <c:crossAx val="94744576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1619,7 +1619,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41306752"/>
+        <c:axId val="94744576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1630,7 +1630,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41305216"/>
+        <c:crossAx val="94734592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1739,8 +1739,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="41354368"/>
-        <c:axId val="41348480"/>
+        <c:axId val="95303936"/>
+        <c:axId val="95302400"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1816,11 +1816,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="41345408"/>
-        <c:axId val="41346944"/>
+        <c:axId val="95294976"/>
+        <c:axId val="95296512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="41345408"/>
+        <c:axId val="95294976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1829,7 +1829,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41346944"/>
+        <c:crossAx val="95296512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1837,7 +1837,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41346944"/>
+        <c:axId val="95296512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.33000000000000007"/>
@@ -1850,12 +1850,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41345408"/>
+        <c:crossAx val="95294976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="41348480"/>
+        <c:axId val="95302400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1865,12 +1865,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41354368"/>
+        <c:crossAx val="95303936"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="41354368"/>
+        <c:axId val="95303936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1879,7 +1879,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41348480"/>
+        <c:crossAx val="95302400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2059,11 +2059,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="40961920"/>
-        <c:axId val="40963456"/>
+        <c:axId val="95358336"/>
+        <c:axId val="95384704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="40961920"/>
+        <c:axId val="95358336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2073,7 +2073,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40963456"/>
+        <c:crossAx val="95384704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2081,7 +2081,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40963456"/>
+        <c:axId val="95384704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2092,13 +2092,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40961920"/>
+        <c:crossAx val="95358336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2356,6 +2357,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2939,7 +2941,7 @@
   <dimension ref="B2:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2950,10 +2952,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="27"/>
+      <c r="B2" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="28"/>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -2984,7 +2986,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" s="2"/>
     </row>
@@ -3008,16 +3010,16 @@
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C10" s="2">
         <v>206</v>
@@ -3035,7 +3037,7 @@
     </row>
     <row r="12" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C12" s="24"/>
     </row>
@@ -3057,11 +3059,11 @@
       <c r="C16" s="25"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -3072,7 +3074,7 @@
         <v>26</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
@@ -3105,7 +3107,7 @@
         <v>28</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
@@ -3131,7 +3133,7 @@
         <v>635</v>
       </c>
       <c r="E26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
@@ -3156,7 +3158,7 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" s="1">
         <v>75</v>
@@ -3166,36 +3168,36 @@
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
+      <c r="B30" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3224,24 +3226,24 @@
   <sheetData>
     <row r="1" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N1" t="s">
+        <v>87</v>
+      </c>
+      <c r="O1" t="s">
         <v>88</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>89</v>
-      </c>
-      <c r="P1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H2">
         <f>O2+O3+O8+O10+O34+O35</f>
@@ -3252,7 +3254,7 @@
         <v>0.27906976744186046</v>
       </c>
       <c r="N2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O2">
         <v>9</v>
@@ -3264,7 +3266,7 @@
     </row>
     <row r="3" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H3">
         <f>O7+O30+O28+O27+O12</f>
@@ -3275,7 +3277,7 @@
         <v>0.12790697674418605</v>
       </c>
       <c r="N3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O3">
         <v>1</v>
@@ -3287,7 +3289,7 @@
     </row>
     <row r="4" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H4">
         <f>O20+O22+O23+O25+O29+O32+O9</f>
@@ -3301,7 +3303,7 @@
     </row>
     <row r="5" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H5">
         <f>O18+O26</f>
@@ -3312,7 +3314,7 @@
         <v>9.3023255813953487E-2</v>
       </c>
       <c r="N5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O5">
         <v>1</v>
@@ -3324,7 +3326,7 @@
     </row>
     <row r="6" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H6">
         <f>SUM(O4,O13)</f>
@@ -3335,7 +3337,7 @@
         <v>1.1627906976744186E-2</v>
       </c>
       <c r="N6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O6">
         <v>1</v>
@@ -3347,7 +3349,7 @@
     </row>
     <row r="7" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H7">
         <f>O15</f>
@@ -3358,7 +3360,7 @@
         <v>0.19767441860465115</v>
       </c>
       <c r="N7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O7">
         <v>2</v>
@@ -3370,7 +3372,7 @@
     </row>
     <row r="8" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H8">
         <f>SUM(O6,O24)</f>
@@ -3381,7 +3383,7 @@
         <v>2.3255813953488372E-2</v>
       </c>
       <c r="N8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O8">
         <v>2</v>
@@ -3393,7 +3395,7 @@
     </row>
     <row r="9" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H9">
         <f>SUM(O33,O5)</f>
@@ -3404,7 +3406,7 @@
         <v>3.4883720930232558E-2</v>
       </c>
       <c r="N9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O9">
         <v>4</v>
@@ -3416,7 +3418,7 @@
     </row>
     <row r="10" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H10">
         <f>SUM(O11,O14,O16,O17,O19,O21,O31)</f>
@@ -3427,7 +3429,7 @@
         <v>9.3023255813953487E-2</v>
       </c>
       <c r="N10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O10">
         <v>1</v>
@@ -3440,7 +3442,7 @@
     <row r="11" spans="7:16" x14ac:dyDescent="0.25">
       <c r="I11" s="6"/>
       <c r="N11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O11">
         <v>1</v>
@@ -3453,7 +3455,7 @@
     <row r="12" spans="7:16" x14ac:dyDescent="0.25">
       <c r="I12" s="6"/>
       <c r="N12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O12">
         <v>2</v>
@@ -3466,7 +3468,7 @@
     <row r="13" spans="7:16" x14ac:dyDescent="0.25">
       <c r="I13" s="6"/>
       <c r="N13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O13">
         <v>1</v>
@@ -3479,7 +3481,7 @@
     <row r="14" spans="7:16" x14ac:dyDescent="0.25">
       <c r="I14" s="6"/>
       <c r="N14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O14">
         <v>1</v>
@@ -3492,7 +3494,7 @@
     <row r="15" spans="7:16" x14ac:dyDescent="0.25">
       <c r="I15" s="6"/>
       <c r="N15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O15">
         <v>17</v>
@@ -3505,7 +3507,7 @@
     <row r="16" spans="7:16" x14ac:dyDescent="0.25">
       <c r="I16" s="6"/>
       <c r="N16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O16">
         <v>1</v>
@@ -3518,7 +3520,7 @@
     <row r="17" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I17" s="6"/>
       <c r="N17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O17">
         <v>1</v>
@@ -3531,7 +3533,7 @@
     <row r="18" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I18" s="6"/>
       <c r="N18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O18">
         <v>1</v>
@@ -3548,7 +3550,7 @@
         <v>0.56976744186046513</v>
       </c>
       <c r="N19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O19">
         <v>1</v>
@@ -3565,7 +3567,7 @@
         <v>49</v>
       </c>
       <c r="N20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O20">
         <v>1</v>
@@ -3578,7 +3580,7 @@
     <row r="21" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I21" s="6"/>
       <c r="N21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O21">
         <v>2</v>
@@ -3591,7 +3593,7 @@
     <row r="22" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I22" s="6"/>
       <c r="N22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O22">
         <v>2</v>
@@ -3604,7 +3606,7 @@
     <row r="23" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I23" s="6"/>
       <c r="N23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O23">
         <v>1</v>
@@ -3617,7 +3619,7 @@
     <row r="24" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I24" s="6"/>
       <c r="N24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O24">
         <v>1</v>
@@ -3630,7 +3632,7 @@
     <row r="25" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I25" s="6"/>
       <c r="N25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O25">
         <v>1</v>
@@ -3643,7 +3645,7 @@
     <row r="26" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I26" s="6"/>
       <c r="N26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O26">
         <v>7</v>
@@ -3656,7 +3658,7 @@
     <row r="27" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I27" s="6"/>
       <c r="N27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O27">
         <v>2</v>
@@ -3669,7 +3671,7 @@
     <row r="28" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I28" s="6"/>
       <c r="N28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O28">
         <v>1</v>
@@ -3682,7 +3684,7 @@
     <row r="29" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I29" s="6"/>
       <c r="N29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O29">
         <v>1</v>
@@ -3695,7 +3697,7 @@
     <row r="30" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I30" s="6"/>
       <c r="N30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O30">
         <v>4</v>
@@ -3708,7 +3710,7 @@
     <row r="31" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I31" s="6"/>
       <c r="N31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O31">
         <v>1</v>
@@ -3721,7 +3723,7 @@
     <row r="32" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I32" s="6"/>
       <c r="N32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O32">
         <v>2</v>
@@ -3734,7 +3736,7 @@
     <row r="33" spans="7:16" x14ac:dyDescent="0.25">
       <c r="I33" s="6"/>
       <c r="N33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O33">
         <v>2</v>
@@ -3747,7 +3749,7 @@
     <row r="34" spans="7:16" x14ac:dyDescent="0.25">
       <c r="I34" s="6"/>
       <c r="N34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O34">
         <v>6</v>
@@ -3760,7 +3762,7 @@
     <row r="35" spans="7:16" x14ac:dyDescent="0.25">
       <c r="I35" s="6"/>
       <c r="N35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O35">
         <v>5</v>
@@ -3772,7 +3774,7 @@
     </row>
     <row r="37" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H37">
         <f>SUM(H2:H35)</f>
@@ -3783,7 +3785,7 @@
         <v>1</v>
       </c>
       <c r="N37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O37">
         <f>SUM(O2:O35)</f>
@@ -3805,7 +3807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
@@ -3817,16 +3819,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" t="s">
         <v>110</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
         <v>111</v>
-      </c>
-      <c r="C1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3935,10 +3937,391 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H23"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="5" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B19" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+      <c r="B20" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H21" s="6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3949,33 +4332,33 @@
   <sheetData>
     <row r="1" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
         <v>113</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>114</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>115</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>116</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>117</v>
       </c>
-      <c r="F1" t="s">
-        <v>118</v>
-      </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2">
         <v>200</v>
@@ -4002,7 +4385,7 @@
     </row>
     <row r="3" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3">
         <v>187</v>
@@ -4025,7 +4408,7 @@
     </row>
     <row r="4" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4">
         <v>176</v>
@@ -4048,7 +4431,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5">
         <v>151</v>
@@ -4070,308 +4453,308 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I6" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
+      <c r="I6" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="30"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="30"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I12" s="30"/>
-      <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="30"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="31"/>
+      <c r="P16" s="31"/>
     </row>
     <row r="17" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
-      <c r="P17" s="30"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="31"/>
     </row>
     <row r="18" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="30"/>
-      <c r="P18" s="30"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="31"/>
     </row>
     <row r="19" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="30"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="30"/>
-      <c r="P19" s="30"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="31"/>
     </row>
     <row r="20" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I20" s="30"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="30"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="30"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
     </row>
     <row r="22" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I22" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
-      <c r="M22" s="31"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="31"/>
-      <c r="P22" s="31"/>
+      <c r="I22" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="32"/>
     </row>
     <row r="23" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
-      <c r="M23" s="31"/>
-      <c r="N23" s="31"/>
-      <c r="O23" s="31"/>
-      <c r="P23" s="31"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="32"/>
     </row>
     <row r="24" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="31"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="31"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="32"/>
     </row>
     <row r="25" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="31"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
     </row>
     <row r="26" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="31"/>
-      <c r="P26" s="31"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="32"/>
     </row>
     <row r="27" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="31"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="32"/>
     </row>
     <row r="28" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="31"/>
-      <c r="O28" s="31"/>
-      <c r="P28" s="31"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="32"/>
     </row>
     <row r="29" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="31"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="32"/>
+      <c r="P29" s="32"/>
     </row>
     <row r="30" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
-      <c r="N30" s="31"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="31"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="32"/>
     </row>
     <row r="31" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="31"/>
-      <c r="M31" s="31"/>
-      <c r="N31" s="31"/>
-      <c r="O31" s="31"/>
-      <c r="P31" s="31"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="32"/>
+      <c r="M31" s="32"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="32"/>
     </row>
     <row r="32" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="31"/>
-      <c r="M32" s="31"/>
-      <c r="N32" s="31"/>
-      <c r="O32" s="31"/>
-      <c r="P32" s="31"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="32"/>
+      <c r="O32" s="32"/>
+      <c r="P32" s="32"/>
     </row>
     <row r="33" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
-      <c r="L33" s="31"/>
-      <c r="M33" s="31"/>
-      <c r="N33" s="31"/>
-      <c r="O33" s="31"/>
-      <c r="P33" s="31"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="32"/>
+      <c r="P33" s="32"/>
     </row>
     <row r="34" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
-      <c r="M34" s="31"/>
-      <c r="N34" s="31"/>
-      <c r="O34" s="31"/>
-      <c r="P34" s="31"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="32"/>
+      <c r="L34" s="32"/>
+      <c r="M34" s="32"/>
+      <c r="N34" s="32"/>
+      <c r="O34" s="32"/>
+      <c r="P34" s="32"/>
     </row>
     <row r="35" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="31"/>
-      <c r="M35" s="31"/>
-      <c r="N35" s="31"/>
-      <c r="O35" s="31"/>
-      <c r="P35" s="31"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="32"/>
+      <c r="L35" s="32"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="32"/>
+      <c r="O35" s="32"/>
+      <c r="P35" s="32"/>
     </row>
     <row r="36" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
-      <c r="L36" s="31"/>
-      <c r="M36" s="31"/>
-      <c r="N36" s="31"/>
-      <c r="O36" s="31"/>
-      <c r="P36" s="31"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="32"/>
+      <c r="L36" s="32"/>
+      <c r="M36" s="32"/>
+      <c r="N36" s="32"/>
+      <c r="O36" s="32"/>
+      <c r="P36" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4380,387 +4763,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H23"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="5" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18">
-        <v>0.67</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B19" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="2:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="B20" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="H21" s="6">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4779,7 +4781,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -4787,7 +4789,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>2.6</v>
@@ -4798,7 +4800,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>4.1100000000000003</v>
@@ -4809,7 +4811,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>0.83</v>
@@ -4820,7 +4822,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <f>B4+B5</f>
@@ -4833,7 +4835,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7">
         <f>B4-B5</f>
@@ -4846,7 +4848,7 @@
     </row>
     <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="6">
         <f>(B3-B4)/B4</f>
@@ -4859,7 +4861,7 @@
     </row>
     <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="6">
         <f>(B3-B6)/B6</f>
@@ -4872,7 +4874,7 @@
     </row>
     <row r="22" spans="5:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="5:6" ht="14.45" x14ac:dyDescent="0.3">
@@ -4902,18 +4904,18 @@
   <sheetData>
     <row r="1" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M1" t="s">
+        <v>87</v>
+      </c>
+      <c r="N1" t="s">
         <v>88</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>89</v>
-      </c>
-      <c r="O1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N2">
         <v>9</v>
@@ -4925,7 +4927,7 @@
     </row>
     <row r="3" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -4937,7 +4939,7 @@
     </row>
     <row r="4" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O4" s="6">
         <f t="shared" si="0"/>
@@ -4946,7 +4948,7 @@
     </row>
     <row r="5" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -4958,7 +4960,7 @@
     </row>
     <row r="6" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -4970,7 +4972,7 @@
     </row>
     <row r="7" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N7">
         <v>2</v>
@@ -4982,7 +4984,7 @@
     </row>
     <row r="8" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N8">
         <v>2</v>
@@ -4994,7 +4996,7 @@
     </row>
     <row r="9" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N9">
         <v>4</v>
@@ -5006,7 +5008,7 @@
     </row>
     <row r="10" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -5018,7 +5020,7 @@
     </row>
     <row r="11" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -5030,7 +5032,7 @@
     </row>
     <row r="12" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N12">
         <v>2</v>
@@ -5042,7 +5044,7 @@
     </row>
     <row r="13" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -5054,7 +5056,7 @@
     </row>
     <row r="14" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -5066,7 +5068,7 @@
     </row>
     <row r="15" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N15">
         <v>17</v>
@@ -5078,7 +5080,7 @@
     </row>
     <row r="16" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N16">
         <v>1</v>
@@ -5090,7 +5092,7 @@
     </row>
     <row r="17" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N17">
         <v>1</v>
@@ -5102,7 +5104,7 @@
     </row>
     <row r="18" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N18">
         <v>1</v>
@@ -5114,7 +5116,7 @@
     </row>
     <row r="19" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N19">
         <v>1</v>
@@ -5126,7 +5128,7 @@
     </row>
     <row r="20" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N20">
         <v>1</v>
@@ -5138,7 +5140,7 @@
     </row>
     <row r="21" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N21">
         <v>2</v>
@@ -5150,7 +5152,7 @@
     </row>
     <row r="22" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N22">
         <v>2</v>
@@ -5162,7 +5164,7 @@
     </row>
     <row r="23" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N23">
         <v>1</v>
@@ -5174,7 +5176,7 @@
     </row>
     <row r="24" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N24">
         <v>1</v>
@@ -5186,7 +5188,7 @@
     </row>
     <row r="25" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N25">
         <v>1</v>
@@ -5198,7 +5200,7 @@
     </row>
     <row r="26" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N26">
         <v>7</v>
@@ -5210,7 +5212,7 @@
     </row>
     <row r="27" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N27">
         <v>2</v>
@@ -5222,7 +5224,7 @@
     </row>
     <row r="28" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N28">
         <v>1</v>
@@ -5234,7 +5236,7 @@
     </row>
     <row r="29" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N29">
         <v>1</v>
@@ -5246,7 +5248,7 @@
     </row>
     <row r="30" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N30">
         <v>4</v>
@@ -5258,7 +5260,7 @@
     </row>
     <row r="31" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N31">
         <v>1</v>
@@ -5270,7 +5272,7 @@
     </row>
     <row r="32" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N32">
         <v>2</v>
@@ -5282,7 +5284,7 @@
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N33">
         <v>2</v>
@@ -5294,7 +5296,7 @@
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N34">
         <v>6</v>
@@ -5306,7 +5308,7 @@
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N35">
         <v>5</v>
@@ -5318,7 +5320,7 @@
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N37">
         <f>SUM(N2:N35)</f>
@@ -5331,7 +5333,7 @@
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated minor codes and figures
</commit_message>
<xml_diff>
--- a/Paper/excel figures.xlsx
+++ b/Paper/excel figures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="105" windowWidth="15570" windowHeight="8730" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="105" windowWidth="15570" windowHeight="8730"/>
   </bookViews>
   <sheets>
     <sheet name="General Model Stats" sheetId="2" r:id="rId1"/>
@@ -1100,11 +1100,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="46058112"/>
-        <c:axId val="46059904"/>
+        <c:axId val="103459840"/>
+        <c:axId val="103473920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="46058112"/>
+        <c:axId val="103459840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1114,7 +1114,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46059904"/>
+        <c:crossAx val="103473920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1122,7 +1122,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46059904"/>
+        <c:axId val="103473920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1133,14 +1133,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46058112"/>
+        <c:crossAx val="103459840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1242,8 +1241,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="44927616"/>
-        <c:axId val="44926080"/>
+        <c:axId val="103517184"/>
+        <c:axId val="103515648"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1319,11 +1318,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="44918656"/>
-        <c:axId val="44920192"/>
+        <c:axId val="103508224"/>
+        <c:axId val="103514112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44918656"/>
+        <c:axId val="103508224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1332,7 +1331,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44920192"/>
+        <c:crossAx val="103514112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1340,7 +1339,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44920192"/>
+        <c:axId val="103514112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1353,12 +1352,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44918656"/>
+        <c:crossAx val="103508224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="44926080"/>
+        <c:axId val="103515648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1370,12 +1369,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44927616"/>
+        <c:crossAx val="103517184"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="44927616"/>
+        <c:axId val="103517184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1384,7 +1383,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44926080"/>
+        <c:crossAx val="103515648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1394,7 +1393,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1652,7 +1650,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1789,11 +1786,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="131784064"/>
-        <c:axId val="43910272"/>
+        <c:axId val="103620608"/>
+        <c:axId val="103622144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="131784064"/>
+        <c:axId val="103620608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1802,7 +1799,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43910272"/>
+        <c:crossAx val="103622144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1810,7 +1807,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43910272"/>
+        <c:axId val="103622144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1838,21 +1835,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="131784064"/>
+        <c:crossAx val="103620608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2066,11 +2061,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="43939328"/>
-        <c:axId val="43958272"/>
+        <c:axId val="103663488"/>
+        <c:axId val="103670144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43939328"/>
+        <c:axId val="103663488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -2094,19 +2089,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43958272"/>
+        <c:crossAx val="103670144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="43958272"/>
+        <c:axId val="103670144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2134,21 +2128,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43939328"/>
+        <c:crossAx val="103663488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2318,11 +2310,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="46174208"/>
-        <c:axId val="46175744"/>
+        <c:axId val="103870848"/>
+        <c:axId val="103872384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="46174208"/>
+        <c:axId val="103870848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2332,7 +2324,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46175744"/>
+        <c:crossAx val="103872384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2340,7 +2332,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46175744"/>
+        <c:axId val="103872384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2351,14 +2343,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46174208"/>
+        <c:crossAx val="103870848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2895,10 +2886,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E35"/>
+  <dimension ref="B2:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2916,92 +2907,91 @@
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2">
+        <v>540</v>
+      </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C4" s="2">
-        <v>540</v>
+        <v>31</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="2">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>106</v>
+        <v>31</v>
+      </c>
+      <c r="C6" s="2">
+        <v>259</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2">
-        <v>259</v>
+        <v>586</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="2">
-        <v>586</v>
+        <v>51</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>107</v>
+        <v>52</v>
+      </c>
+      <c r="C9" s="2">
+        <v>206</v>
       </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="2">
-        <v>206</v>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1">
+        <v>500</v>
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="1">
-        <v>500</v>
-      </c>
-      <c r="D11" s="2"/>
+    <row r="11" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="24"/>
     </row>
     <row r="12" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" s="24"/>
-    </row>
-    <row r="13" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
-      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="25"/>
@@ -3011,125 +3001,126 @@
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="3"/>
+      <c r="B20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>122</v>
+      <c r="B21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="2">
+        <v>518</v>
+      </c>
+      <c r="D21" s="2">
+        <v>540</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C22" s="2">
-        <v>518</v>
+        <v>30</v>
       </c>
       <c r="D22" s="2">
-        <v>540</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="2">
-        <v>30</v>
-      </c>
-      <c r="D23" s="2">
-        <v>31</v>
+        <v>27</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>106</v>
+        <v>31</v>
+      </c>
+      <c r="C24" s="2">
+        <v>163</v>
+      </c>
+      <c r="D24" s="2">
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C25" s="2">
-        <v>163</v>
+        <v>570</v>
       </c>
       <c r="D25" s="2">
-        <v>259</v>
+        <f>49+586</f>
+        <v>635</v>
+      </c>
+      <c r="E25" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C26" s="2">
-        <v>570</v>
+        <v>49</v>
       </c>
       <c r="D26" s="2">
-        <f>49+586</f>
-        <v>635</v>
-      </c>
-      <c r="E26" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C27" s="2">
-        <v>49</v>
-      </c>
-      <c r="D27" s="2">
-        <v>59</v>
-      </c>
+        <v>464</v>
+      </c>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="2">
-        <v>464</v>
-      </c>
-      <c r="D28" s="2"/>
+      <c r="B28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="1">
+        <v>75</v>
+      </c>
+      <c r="D28" s="8">
+        <v>85</v>
+      </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="1">
-        <v>75</v>
-      </c>
-      <c r="D29" s="8">
-        <v>85</v>
-      </c>
+      <c r="B29" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="30"/>
@@ -3151,16 +3142,11 @@
       <c r="C34" s="30"/>
       <c r="D34" s="30"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B30:D35"/>
+    <mergeCell ref="B29:D34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3764,8 +3750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated model and added thermo demo
</commit_message>
<xml_diff>
--- a/Paper/excel figures.xlsx
+++ b/Paper/excel figures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="105" windowWidth="15570" windowHeight="8730"/>
+    <workbookView xWindow="390" yWindow="105" windowWidth="15570" windowHeight="8730" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="General Model Stats" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="127">
   <si>
     <t>Formate</t>
   </si>
@@ -170,9 +170,6 @@
     <t>Figure 1. Comparison of predicted and experimental growth yields</t>
   </si>
   <si>
-    <t>1 of 2</t>
-  </si>
-  <si>
     <t>∆hdrB2</t>
   </si>
   <si>
@@ -405,9 +402,6 @@
     <t>Genotype</t>
   </si>
   <si>
-    <t>27 of 30</t>
-  </si>
-  <si>
     <t>658/53</t>
   </si>
   <si>
@@ -469,6 +463,12 @@
   </si>
   <si>
     <t>Figure S2: Accuracy and Matthews Correlation Coefficient (MCC) o</t>
+  </si>
+  <si>
+    <t>657/53</t>
+  </si>
+  <si>
+    <t>28 of 30</t>
   </si>
 </sst>
 </file>
@@ -686,7 +686,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -790,7 +790,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8</c:v>
@@ -799,7 +799,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2</c:v>
@@ -808,7 +808,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -905,16 +905,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>200</c:v>
+                  <c:v>198</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>187</c:v>
+                  <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>176</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>151</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -962,16 +962,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>147</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>165</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>173</c:v>
+                  <c:v>172</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>180</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1019,13 +1019,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>110</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>123</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>134</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>159</c:v>
@@ -1076,16 +1076,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>81</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1100,11 +1100,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="103459840"/>
-        <c:axId val="103473920"/>
+        <c:axId val="103332480"/>
+        <c:axId val="103338368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="103459840"/>
+        <c:axId val="103332480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1114,7 +1114,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103473920"/>
+        <c:crossAx val="103338368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1122,7 +1122,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103473920"/>
+        <c:axId val="103338368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1133,13 +1133,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103459840"/>
+        <c:crossAx val="103332480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1217,13 +1218,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>64.3</c:v>
+                  <c:v>64.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65.2</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64.7</c:v>
+                  <c:v>64.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>61.3</c:v>
@@ -1241,8 +1242,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="103517184"/>
-        <c:axId val="103515648"/>
+        <c:axId val="104557184"/>
+        <c:axId val="104555648"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1292,16 +1293,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.28699999999999998</c:v>
+                  <c:v>0.27800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32400000000000001</c:v>
+                  <c:v>0.315</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.32600000000000001</c:v>
+                  <c:v>0.317</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.28299999999999997</c:v>
+                  <c:v>0.27700000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1318,11 +1319,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="103508224"/>
-        <c:axId val="103514112"/>
+        <c:axId val="104548224"/>
+        <c:axId val="104549760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="103508224"/>
+        <c:axId val="104548224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1331,7 +1332,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103514112"/>
+        <c:crossAx val="104549760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1339,7 +1340,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103514112"/>
+        <c:axId val="104549760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1352,12 +1353,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103508224"/>
+        <c:crossAx val="104548224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103515648"/>
+        <c:axId val="104555648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1369,12 +1370,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103517184"/>
+        <c:crossAx val="104557184"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="103517184"/>
+        <c:axId val="104557184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1383,7 +1384,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103515648"/>
+        <c:crossAx val="104555648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1393,6 +1394,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1786,11 +1788,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="103620608"/>
-        <c:axId val="103622144"/>
+        <c:axId val="104697856"/>
+        <c:axId val="104699392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="103620608"/>
+        <c:axId val="104697856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1799,7 +1801,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103622144"/>
+        <c:crossAx val="104699392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1807,7 +1809,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103622144"/>
+        <c:axId val="104699392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1841,7 +1843,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103620608"/>
+        <c:crossAx val="104697856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2061,11 +2063,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="103663488"/>
-        <c:axId val="103670144"/>
+        <c:axId val="106247680"/>
+        <c:axId val="106258432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="103663488"/>
+        <c:axId val="106247680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -2095,12 +2097,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103670144"/>
+        <c:crossAx val="106258432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="103670144"/>
+        <c:axId val="106258432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2134,7 +2136,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103663488"/>
+        <c:crossAx val="106247680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2310,11 +2312,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="103870848"/>
-        <c:axId val="103872384"/>
+        <c:axId val="106288640"/>
+        <c:axId val="106290176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="103870848"/>
+        <c:axId val="106288640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2324,7 +2326,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103872384"/>
+        <c:crossAx val="106290176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2332,7 +2334,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103872384"/>
+        <c:axId val="106290176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2343,7 +2345,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="103870848"/>
+        <c:crossAx val="106288640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2888,8 +2890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2901,7 +2903,7 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="28"/>
       <c r="D2" s="7"/>
@@ -2911,7 +2913,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="2">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D3" s="2"/>
     </row>
@@ -2929,7 +2931,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -2938,7 +2940,7 @@
         <v>31</v>
       </c>
       <c r="C6" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D6" s="2"/>
     </row>
@@ -2947,22 +2949,22 @@
         <v>21</v>
       </c>
       <c r="C7" s="2">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2">
         <v>206</v>
@@ -2974,13 +2976,13 @@
         <v>23</v>
       </c>
       <c r="C10" s="1">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C11" s="24"/>
     </row>
@@ -3017,7 +3019,7 @@
         <v>26</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -3050,7 +3052,7 @@
         <v>28</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -3076,7 +3078,7 @@
         <v>635</v>
       </c>
       <c r="E25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -3101,7 +3103,7 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" s="1">
         <v>75</v>
@@ -3112,7 +3114,7 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C29" s="29"/>
       <c r="D29" s="29"/>
@@ -3158,7 +3160,7 @@
   <dimension ref="G1:P37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3169,24 +3171,24 @@
   <sheetData>
     <row r="1" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N1" t="s">
+        <v>86</v>
+      </c>
+      <c r="O1" t="s">
         <v>87</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>88</v>
-      </c>
-      <c r="P1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H2">
         <f>O2+O3+O8+O10+O34+O35</f>
@@ -3197,19 +3199,19 @@
         <v>0.27906976744186046</v>
       </c>
       <c r="N2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O2">
         <v>9</v>
       </c>
       <c r="P2" s="6">
         <f>O2/$O$37</f>
-        <v>0.10465116279069768</v>
+        <v>0.10843373493975904</v>
       </c>
     </row>
     <row r="3" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H3">
         <f>O7+O30+O28+O27+O12</f>
@@ -3220,33 +3222,33 @@
         <v>0.12790697674418605</v>
       </c>
       <c r="N3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O3">
         <v>1</v>
       </c>
       <c r="P3" s="6">
         <f t="shared" ref="P3:P35" si="1">O3/$O$37</f>
-        <v>1.1627906976744186E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="4" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H4">
         <f>O20+O22+O23+O25+O29+O32+O9</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I4" s="6">
         <f t="shared" si="0"/>
-        <v>0.13953488372093023</v>
+        <v>0.12790697674418605</v>
       </c>
       <c r="P4" s="6"/>
     </row>
     <row r="5" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H5">
         <f>O18+O26</f>
@@ -3257,19 +3259,19 @@
         <v>9.3023255813953487E-2</v>
       </c>
       <c r="N5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O5">
         <v>1</v>
       </c>
       <c r="P5" s="6">
         <f t="shared" si="1"/>
-        <v>1.1627906976744186E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="6" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H6">
         <f>SUM(O4,O13)</f>
@@ -3280,42 +3282,42 @@
         <v>1.1627906976744186E-2</v>
       </c>
       <c r="N6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O6">
         <v>1</v>
       </c>
       <c r="P6" s="6">
         <f t="shared" si="1"/>
-        <v>1.1627906976744186E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="7" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H7">
         <f>O15</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I7" s="6">
         <f t="shared" si="0"/>
-        <v>0.19767441860465115</v>
+        <v>0.18604651162790697</v>
       </c>
       <c r="N7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O7">
         <v>2</v>
       </c>
       <c r="P7" s="6">
         <f t="shared" si="1"/>
-        <v>2.3255813953488372E-2</v>
+        <v>2.4096385542168676E-2</v>
       </c>
     </row>
     <row r="8" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H8">
         <f>SUM(O6,O24)</f>
@@ -3326,19 +3328,19 @@
         <v>2.3255813953488372E-2</v>
       </c>
       <c r="N8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O8">
         <v>2</v>
       </c>
       <c r="P8" s="6">
         <f t="shared" si="1"/>
-        <v>2.3255813953488372E-2</v>
+        <v>2.4096385542168676E-2</v>
       </c>
     </row>
     <row r="9" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H9">
         <f>SUM(O33,O5)</f>
@@ -3349,394 +3351,385 @@
         <v>3.4883720930232558E-2</v>
       </c>
       <c r="N9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O9">
         <v>4</v>
       </c>
       <c r="P9" s="6">
         <f t="shared" si="1"/>
-        <v>4.6511627906976744E-2</v>
+        <v>4.8192771084337352E-2</v>
       </c>
     </row>
     <row r="10" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H10">
         <f>SUM(O11,O14,O16,O17,O19,O21,O31)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I10" s="6">
         <f t="shared" si="0"/>
-        <v>9.3023255813953487E-2</v>
+        <v>8.1395348837209308E-2</v>
       </c>
       <c r="N10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O10">
         <v>1</v>
       </c>
       <c r="P10" s="6">
         <f t="shared" si="1"/>
-        <v>1.1627906976744186E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="11" spans="7:16" x14ac:dyDescent="0.25">
       <c r="I11" s="6"/>
       <c r="N11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O11">
         <v>1</v>
       </c>
       <c r="P11" s="6">
         <f t="shared" si="1"/>
-        <v>1.1627906976744186E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="12" spans="7:16" x14ac:dyDescent="0.25">
       <c r="I12" s="6"/>
       <c r="N12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O12">
         <v>2</v>
       </c>
       <c r="P12" s="6">
         <f t="shared" si="1"/>
-        <v>2.3255813953488372E-2</v>
+        <v>2.4096385542168676E-2</v>
       </c>
     </row>
     <row r="13" spans="7:16" x14ac:dyDescent="0.25">
       <c r="I13" s="6"/>
       <c r="N13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O13">
         <v>1</v>
       </c>
       <c r="P13" s="6">
         <f t="shared" si="1"/>
-        <v>1.1627906976744186E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="14" spans="7:16" x14ac:dyDescent="0.25">
       <c r="I14" s="6"/>
-      <c r="N14" t="s">
-        <v>74</v>
-      </c>
-      <c r="O14">
-        <v>1</v>
-      </c>
-      <c r="P14" s="6">
-        <f t="shared" si="1"/>
-        <v>1.1627906976744186E-2</v>
-      </c>
+      <c r="P14" s="6"/>
     </row>
     <row r="15" spans="7:16" x14ac:dyDescent="0.25">
       <c r="I15" s="6"/>
       <c r="N15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O15">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P15" s="6">
         <f t="shared" si="1"/>
-        <v>0.19767441860465115</v>
+        <v>0.19277108433734941</v>
       </c>
     </row>
     <row r="16" spans="7:16" x14ac:dyDescent="0.25">
       <c r="I16" s="6"/>
       <c r="N16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O16">
         <v>1</v>
       </c>
       <c r="P16" s="6">
         <f t="shared" si="1"/>
-        <v>1.1627906976744186E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="17" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I17" s="6"/>
       <c r="N17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O17">
         <v>1</v>
       </c>
       <c r="P17" s="6">
         <f t="shared" si="1"/>
-        <v>1.1627906976744186E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="18" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I18" s="6"/>
       <c r="N18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O18">
         <v>1</v>
       </c>
       <c r="P18" s="6">
         <f t="shared" si="1"/>
-        <v>1.1627906976744186E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="19" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I19" s="6"/>
       <c r="K19">
         <f>SUM(H3,H4,H5,H6,H7)/86</f>
-        <v>0.56976744186046513</v>
+        <v>0.54651162790697672</v>
       </c>
       <c r="N19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O19">
         <v>1</v>
       </c>
       <c r="P19" s="6">
         <f t="shared" si="1"/>
-        <v>1.1627906976744186E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="20" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I20" s="6"/>
       <c r="K20">
         <f>K19*86</f>
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O20">
         <v>1</v>
       </c>
       <c r="P20" s="6">
         <f t="shared" si="1"/>
-        <v>1.1627906976744186E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="21" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I21" s="6"/>
       <c r="N21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O21">
         <v>2</v>
       </c>
       <c r="P21" s="6">
         <f t="shared" si="1"/>
-        <v>2.3255813953488372E-2</v>
+        <v>2.4096385542168676E-2</v>
       </c>
     </row>
     <row r="22" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I22" s="6"/>
       <c r="N22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P22" s="6">
         <f t="shared" si="1"/>
-        <v>2.3255813953488372E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="23" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I23" s="6"/>
       <c r="N23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O23">
         <v>1</v>
       </c>
       <c r="P23" s="6">
         <f t="shared" si="1"/>
-        <v>1.1627906976744186E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="24" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I24" s="6"/>
       <c r="N24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O24">
         <v>1</v>
       </c>
       <c r="P24" s="6">
         <f t="shared" si="1"/>
-        <v>1.1627906976744186E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="25" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I25" s="6"/>
       <c r="N25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O25">
         <v>1</v>
       </c>
       <c r="P25" s="6">
         <f t="shared" si="1"/>
-        <v>1.1627906976744186E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="26" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I26" s="6"/>
       <c r="N26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O26">
         <v>7</v>
       </c>
       <c r="P26" s="6">
         <f t="shared" si="1"/>
-        <v>8.1395348837209308E-2</v>
+        <v>8.4337349397590355E-2</v>
       </c>
     </row>
     <row r="27" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I27" s="6"/>
       <c r="N27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O27">
         <v>2</v>
       </c>
       <c r="P27" s="6">
         <f t="shared" si="1"/>
-        <v>2.3255813953488372E-2</v>
+        <v>2.4096385542168676E-2</v>
       </c>
     </row>
     <row r="28" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I28" s="6"/>
       <c r="N28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O28">
         <v>1</v>
       </c>
       <c r="P28" s="6">
         <f t="shared" si="1"/>
-        <v>1.1627906976744186E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="29" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I29" s="6"/>
       <c r="N29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O29">
         <v>1</v>
       </c>
       <c r="P29" s="6">
         <f t="shared" si="1"/>
-        <v>1.1627906976744186E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="30" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I30" s="6"/>
       <c r="N30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O30">
         <v>4</v>
       </c>
       <c r="P30" s="6">
         <f t="shared" si="1"/>
-        <v>4.6511627906976744E-2</v>
+        <v>4.8192771084337352E-2</v>
       </c>
     </row>
     <row r="31" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I31" s="6"/>
       <c r="N31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O31">
         <v>1</v>
       </c>
       <c r="P31" s="6">
         <f t="shared" si="1"/>
-        <v>1.1627906976744186E-2</v>
+        <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="32" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I32" s="6"/>
       <c r="N32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O32">
         <v>2</v>
       </c>
       <c r="P32" s="6">
         <f t="shared" si="1"/>
-        <v>2.3255813953488372E-2</v>
+        <v>2.4096385542168676E-2</v>
       </c>
     </row>
     <row r="33" spans="7:16" x14ac:dyDescent="0.25">
       <c r="I33" s="6"/>
       <c r="N33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O33">
         <v>2</v>
       </c>
       <c r="P33" s="6">
         <f t="shared" si="1"/>
-        <v>2.3255813953488372E-2</v>
+        <v>2.4096385542168676E-2</v>
       </c>
     </row>
     <row r="34" spans="7:16" x14ac:dyDescent="0.25">
       <c r="I34" s="6"/>
       <c r="N34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O34">
         <v>6</v>
       </c>
       <c r="P34" s="6">
         <f t="shared" si="1"/>
-        <v>6.9767441860465115E-2</v>
+        <v>7.2289156626506021E-2</v>
       </c>
     </row>
     <row r="35" spans="7:16" x14ac:dyDescent="0.25">
       <c r="I35" s="6"/>
       <c r="N35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O35">
         <v>5</v>
       </c>
       <c r="P35" s="6">
         <f t="shared" si="1"/>
-        <v>5.8139534883720929E-2</v>
+        <v>6.0240963855421686E-2</v>
       </c>
     </row>
     <row r="37" spans="7:16" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H37">
         <f>SUM(H2:H35)</f>
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I37" s="6">
         <f>SUM(I2:I35)</f>
-        <v>1</v>
+        <v>0.96511627906976749</v>
       </c>
       <c r="N37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O37">
         <f>SUM(O2:O35)</f>
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="P37">
         <f>SUM(P2:P35)</f>
-        <v>1.0000000000000004</v>
+        <v>1.0000000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -3751,7 +3744,7 @@
   <dimension ref="B2:H23"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3762,7 +3755,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>2</v>
@@ -3881,7 +3874,7 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>32</v>
@@ -4032,7 +4025,7 @@
         <v>32</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -4049,15 +4042,15 @@
         <v>32</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H18">
-        <v>0.67</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>32</v>
@@ -4075,7 +4068,7 @@
     </row>
     <row r="20" spans="2:8" ht="18" x14ac:dyDescent="0.35">
       <c r="B20" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>32</v>
@@ -4098,27 +4091,27 @@
         <v>34</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="H21" s="6">
-        <v>0.9</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -4131,8 +4124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4143,129 +4136,129 @@
   <sheetData>
     <row r="1" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
         <v>112</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>113</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>114</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>115</v>
       </c>
-      <c r="E1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F1" t="s">
-        <v>117</v>
-      </c>
       <c r="G1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C2">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F2">
-        <v>64.3</v>
+        <v>64.099999999999994</v>
       </c>
       <c r="G2">
-        <v>0.28699999999999998</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="H2">
         <f>SUM(B2:E2)</f>
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B3">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C3">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D3">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E3">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F3">
-        <v>65.2</v>
+        <v>65</v>
       </c>
       <c r="G3">
-        <v>0.32400000000000001</v>
+        <v>0.315</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B4">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C4">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D4">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E4">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F4">
-        <v>64.7</v>
+        <v>64.400000000000006</v>
       </c>
       <c r="G4">
-        <v>0.32600000000000001</v>
+        <v>0.317</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D5">
         <v>159</v>
       </c>
       <c r="E5">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F5">
         <v>61.3</v>
       </c>
       <c r="G5">
-        <v>0.28299999999999997</v>
+        <v>0.27700000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I6" s="31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J6" s="31"/>
       <c r="K6" s="31"/>
@@ -4417,7 +4410,7 @@
     </row>
     <row r="22" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I22" s="32" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
@@ -4582,7 +4575,7 @@
   <dimension ref="B1:O40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:O37"/>
+      <selection activeCell="J71" sqref="J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4592,18 +4585,18 @@
   <sheetData>
     <row r="1" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M1" t="s">
+        <v>86</v>
+      </c>
+      <c r="N1" t="s">
         <v>87</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>88</v>
-      </c>
-      <c r="O1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N2">
         <v>9</v>
@@ -4615,7 +4608,7 @@
     </row>
     <row r="3" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -4627,7 +4620,7 @@
     </row>
     <row r="4" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O4" s="6">
         <f t="shared" si="0"/>
@@ -4636,7 +4629,7 @@
     </row>
     <row r="5" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -4648,7 +4641,7 @@
     </row>
     <row r="6" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -4660,7 +4653,7 @@
     </row>
     <row r="7" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N7">
         <v>2</v>
@@ -4672,7 +4665,7 @@
     </row>
     <row r="8" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N8">
         <v>2</v>
@@ -4684,7 +4677,7 @@
     </row>
     <row r="9" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N9">
         <v>4</v>
@@ -4696,7 +4689,7 @@
     </row>
     <row r="10" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -4708,7 +4701,7 @@
     </row>
     <row r="11" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -4720,7 +4713,7 @@
     </row>
     <row r="12" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N12">
         <v>2</v>
@@ -4732,7 +4725,7 @@
     </row>
     <row r="13" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -4744,7 +4737,7 @@
     </row>
     <row r="14" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -4756,7 +4749,7 @@
     </row>
     <row r="15" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N15">
         <v>17</v>
@@ -4768,7 +4761,7 @@
     </row>
     <row r="16" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N16">
         <v>1</v>
@@ -4780,7 +4773,7 @@
     </row>
     <row r="17" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N17">
         <v>1</v>
@@ -4792,7 +4785,7 @@
     </row>
     <row r="18" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N18">
         <v>1</v>
@@ -4804,7 +4797,7 @@
     </row>
     <row r="19" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N19">
         <v>1</v>
@@ -4816,7 +4809,7 @@
     </row>
     <row r="20" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N20">
         <v>1</v>
@@ -4828,7 +4821,7 @@
     </row>
     <row r="21" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N21">
         <v>2</v>
@@ -4840,7 +4833,7 @@
     </row>
     <row r="22" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N22">
         <v>2</v>
@@ -4852,7 +4845,7 @@
     </row>
     <row r="23" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N23">
         <v>1</v>
@@ -4864,7 +4857,7 @@
     </row>
     <row r="24" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N24">
         <v>1</v>
@@ -4876,7 +4869,7 @@
     </row>
     <row r="25" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N25">
         <v>1</v>
@@ -4888,7 +4881,7 @@
     </row>
     <row r="26" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N26">
         <v>7</v>
@@ -4900,7 +4893,7 @@
     </row>
     <row r="27" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N27">
         <v>2</v>
@@ -4912,7 +4905,7 @@
     </row>
     <row r="28" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N28">
         <v>1</v>
@@ -4924,7 +4917,7 @@
     </row>
     <row r="29" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N29">
         <v>1</v>
@@ -4936,7 +4929,7 @@
     </row>
     <row r="30" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N30">
         <v>4</v>
@@ -4948,7 +4941,7 @@
     </row>
     <row r="31" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N31">
         <v>1</v>
@@ -4960,7 +4953,7 @@
     </row>
     <row r="32" spans="13:15" x14ac:dyDescent="0.25">
       <c r="M32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N32">
         <v>2</v>
@@ -4972,7 +4965,7 @@
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N33">
         <v>2</v>
@@ -4984,7 +4977,7 @@
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N34">
         <v>6</v>
@@ -4996,7 +4989,7 @@
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N35">
         <v>5</v>
@@ -5008,7 +5001,7 @@
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="M37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N37">
         <f>SUM(N2:N35)</f>
@@ -5021,7 +5014,7 @@
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -5047,16 +5040,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C1" t="s">
         <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5245,7 +5238,7 @@
     </row>
     <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="6">
         <f>(B3-B4)/B4</f>
@@ -5258,7 +5251,7 @@
     </row>
     <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="6">
         <f>(B3-B6)/B6</f>

</xml_diff>